<commit_message>
regen save_data to use K instead of Strike#, regen std/mean, calc and write s_vals
</commit_message>
<xml_diff>
--- a/data/calcs/save_calcs/2024_mean_data.xlsx
+++ b/data/calcs/save_calcs/2024_mean_data.xlsx
@@ -509,7 +509,7 @@
         <v>2.333333333333333</v>
       </c>
       <c r="F3" t="n">
-        <v>4.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -540,7 +540,7 @@
         <v>1.384615384615385</v>
       </c>
       <c r="F4" t="n">
-        <v>5.384615384615385</v>
+        <v>1.384615384615385</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -571,7 +571,7 @@
         <v>-2</v>
       </c>
       <c r="F5" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -602,7 +602,7 @@
         <v>-1.333333333333333</v>
       </c>
       <c r="F6" t="n">
-        <v>4.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -633,7 +633,7 @@
         <v>1.3125</v>
       </c>
       <c r="F7" t="n">
-        <v>5.9375</v>
+        <v>1.375</v>
       </c>
       <c r="G7" t="n">
         <v>1.1875</v>
@@ -664,7 +664,7 @@
         <v>-1.5</v>
       </c>
       <c r="F8" t="n">
-        <v>8.166666666666666</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G8" t="n">
         <v>1.5</v>
@@ -695,7 +695,7 @@
         <v>-1.5</v>
       </c>
       <c r="F9" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>1.166666666666667</v>
@@ -726,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
         <v>1.5</v>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -788,7 +788,7 @@
         <v>2.043478260869565</v>
       </c>
       <c r="F12" t="n">
-        <v>4.956521739130435</v>
+        <v>1.217391304347826</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
@@ -819,7 +819,7 @@
         <v>-10</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -850,7 +850,7 @@
         <v>1.454545454545455</v>
       </c>
       <c r="F14" t="n">
-        <v>5.090909090909091</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="G14" t="n">
         <v>1.090909090909091</v>
@@ -881,7 +881,7 @@
         <v>-1.1875</v>
       </c>
       <c r="F15" t="n">
-        <v>10.3125</v>
+        <v>1.6875</v>
       </c>
       <c r="G15" t="n">
         <v>2.3125</v>
@@ -912,7 +912,7 @@
         <v>0.8</v>
       </c>
       <c r="F16" t="n">
-        <v>4.4</v>
+        <v>0.7</v>
       </c>
       <c r="G16" t="n">
         <v>1.1</v>
@@ -943,7 +943,7 @@
         <v>2.076923076923077</v>
       </c>
       <c r="F17" t="n">
-        <v>4.615384615384615</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
         <v>1.153846153846154</v>
@@ -974,7 +974,7 @@
         <v>2.125</v>
       </c>
       <c r="F18" t="n">
-        <v>6.25</v>
+        <v>1.25</v>
       </c>
       <c r="G18" t="n">
         <v>1.375</v>
@@ -1005,7 +1005,7 @@
         <v>-1</v>
       </c>
       <c r="F19" t="n">
-        <v>11.66666666666667</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
         <v>4</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="G20" t="n">
         <v>1.5</v>
@@ -1067,7 +1067,7 @@
         <v>-4.333333333333333</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>
@@ -1098,7 +1098,7 @@
         <v>-1.571428571428571</v>
       </c>
       <c r="F22" t="n">
-        <v>4</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="G22" t="n">
         <v>1.285714285714286</v>
@@ -1129,7 +1129,7 @@
         <v>2.5</v>
       </c>
       <c r="F23" t="n">
-        <v>13.5</v>
+        <v>3.5</v>
       </c>
       <c r="G23" t="n">
         <v>2.5</v>
@@ -1160,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>9.199999999999999</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
         <v>1.8</v>
@@ -1191,7 +1191,7 @@
         <v>-3.125</v>
       </c>
       <c r="F25" t="n">
-        <v>5.875</v>
+        <v>1.875</v>
       </c>
       <c r="G25" t="n">
         <v>1.625</v>
@@ -1222,7 +1222,7 @@
         <v>-2.4</v>
       </c>
       <c r="F26" t="n">
-        <v>6.6</v>
+        <v>1.4</v>
       </c>
       <c r="G26" t="n">
         <v>1.4</v>
@@ -1253,7 +1253,7 @@
         <v>-0.1428571428571428</v>
       </c>
       <c r="F27" t="n">
-        <v>4</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="G27" t="n">
         <v>1</v>
@@ -1284,7 +1284,7 @@
         <v>0.6363636363636364</v>
       </c>
       <c r="F28" t="n">
-        <v>5.363636363636363</v>
+        <v>1.272727272727273</v>
       </c>
       <c r="G28" t="n">
         <v>1.181818181818182</v>
@@ -1315,7 +1315,7 @@
         <v>1.416666666666667</v>
       </c>
       <c r="F29" t="n">
-        <v>5.083333333333333</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
         <v>1.083333333333333</v>
@@ -1346,7 +1346,7 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="n">
-        <v>5.166666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>
@@ -1377,7 +1377,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="F31" t="n">
-        <v>4.166666666666667</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
@@ -1408,7 +1408,7 @@
         <v>-10</v>
       </c>
       <c r="F32" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
         <v>1</v>
@@ -1439,7 +1439,7 @@
         <v>1.909090909090909</v>
       </c>
       <c r="F33" t="n">
-        <v>5.272727272727272</v>
+        <v>1.363636363636364</v>
       </c>
       <c r="G33" t="n">
         <v>1.272727272727273</v>
@@ -1470,7 +1470,7 @@
         <v>2.416666666666667</v>
       </c>
       <c r="F34" t="n">
-        <v>5.666666666666667</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G34" t="n">
         <v>1.25</v>
@@ -1501,7 +1501,7 @@
         <v>9.5</v>
       </c>
       <c r="F35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
         <v>1.5</v>
@@ -1532,7 +1532,7 @@
         <v>1.204081632653061</v>
       </c>
       <c r="F36" t="n">
-        <v>4.63265306122449</v>
+        <v>0.8979591836734694</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
@@ -1563,7 +1563,7 @@
         <v>4.5</v>
       </c>
       <c r="F37" t="n">
-        <v>7.5</v>
+        <v>2</v>
       </c>
       <c r="G37" t="n">
         <v>1.5</v>
@@ -1594,7 +1594,7 @@
         <v>0.4615384615384616</v>
       </c>
       <c r="F38" t="n">
-        <v>4.230769230769231</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="G38" t="n">
         <v>1.269230769230769</v>
@@ -1656,7 +1656,7 @@
         <v>-1.625</v>
       </c>
       <c r="F40" t="n">
-        <v>5</v>
+        <v>1.375</v>
       </c>
       <c r="G40" t="n">
         <v>1.25</v>
@@ -1687,7 +1687,7 @@
         <v>-2.5</v>
       </c>
       <c r="F41" t="n">
-        <v>6.5</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
         <v>1.5</v>
@@ -1718,7 +1718,7 @@
         <v>-5</v>
       </c>
       <c r="F42" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G42" t="n">
         <v>2</v>
@@ -1749,7 +1749,7 @@
         <v>-1.75</v>
       </c>
       <c r="F43" t="n">
-        <v>4.75</v>
+        <v>1.25</v>
       </c>
       <c r="G43" t="n">
         <v>1</v>
@@ -1780,7 +1780,7 @@
         <v>-2</v>
       </c>
       <c r="F44" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G44" t="n">
         <v>1.5</v>
@@ -1811,7 +1811,7 @@
         <v>-3.2</v>
       </c>
       <c r="F45" t="n">
-        <v>5.2</v>
+        <v>0.6</v>
       </c>
       <c r="G45" t="n">
         <v>1.6</v>
@@ -1842,7 +1842,7 @@
         <v>-1.142857142857143</v>
       </c>
       <c r="F46" t="n">
-        <v>2.571428571428572</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G46" t="n">
         <v>1.285714285714286</v>
@@ -1873,7 +1873,7 @@
         <v>-5.5</v>
       </c>
       <c r="F47" t="n">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="G47" t="n">
         <v>1</v>
@@ -1904,7 +1904,7 @@
         <v>8</v>
       </c>
       <c r="F48" t="n">
-        <v>24.33333333333333</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="G48" t="n">
         <v>5</v>
@@ -1935,7 +1935,7 @@
         <v>-0.5</v>
       </c>
       <c r="F49" t="n">
-        <v>3.25</v>
+        <v>0.75</v>
       </c>
       <c r="G49" t="n">
         <v>1</v>
@@ -1966,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G50" t="n">
         <v>1.5</v>
@@ -1997,7 +1997,7 @@
         <v>-7</v>
       </c>
       <c r="F51" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
@@ -2028,7 +2028,7 @@
         <v>-0.8333333333333334</v>
       </c>
       <c r="F52" t="n">
-        <v>4.333333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G52" t="n">
         <v>1.166666666666667</v>
@@ -2059,7 +2059,7 @@
         <v>-3.5</v>
       </c>
       <c r="F53" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
         <v>1</v>
@@ -2090,7 +2090,7 @@
         <v>0.5</v>
       </c>
       <c r="F54" t="n">
-        <v>6.75</v>
+        <v>1.5</v>
       </c>
       <c r="G54" t="n">
         <v>1.25</v>
@@ -2121,7 +2121,7 @@
         <v>-1.8</v>
       </c>
       <c r="F55" t="n">
-        <v>4.2</v>
+        <v>1</v>
       </c>
       <c r="G55" t="n">
         <v>1</v>
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>6.833333333333333</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
         <v>1.333333333333333</v>
@@ -2183,7 +2183,7 @@
         <v>1.1</v>
       </c>
       <c r="F57" t="n">
-        <v>6.9</v>
+        <v>1.4</v>
       </c>
       <c r="G57" t="n">
         <v>1.5</v>
@@ -2214,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>6.25</v>
+        <v>1.125</v>
       </c>
       <c r="G58" t="n">
         <v>1.875</v>
@@ -2245,7 +2245,7 @@
         <v>-1.666666666666667</v>
       </c>
       <c r="F59" t="n">
-        <v>5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G59" t="n">
         <v>1.333333333333333</v>
@@ -2276,7 +2276,7 @@
         <v>8</v>
       </c>
       <c r="F60" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G60" t="n">
         <v>5</v>
@@ -2307,7 +2307,7 @@
         <v>-14.5</v>
       </c>
       <c r="F61" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
@@ -2338,7 +2338,7 @@
         <v>1.571428571428571</v>
       </c>
       <c r="F62" t="n">
-        <v>7</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="G62" t="n">
         <v>1.285714285714286</v>
@@ -2369,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G63" t="n">
         <v>1</v>
@@ -2400,7 +2400,7 @@
         <v>-0.25</v>
       </c>
       <c r="F64" t="n">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="G64" t="n">
         <v>1.25</v>
@@ -2431,7 +2431,7 @@
         <v>2.5</v>
       </c>
       <c r="F65" t="n">
-        <v>5</v>
+        <v>1.1</v>
       </c>
       <c r="G65" t="n">
         <v>1</v>
@@ -2462,7 +2462,7 @@
         <v>-2</v>
       </c>
       <c r="F66" t="n">
-        <v>5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G66" t="n">
         <v>1.333333333333333</v>
@@ -2493,7 +2493,7 @@
         <v>3.4</v>
       </c>
       <c r="F67" t="n">
-        <v>4.6</v>
+        <v>1.4</v>
       </c>
       <c r="G67" t="n">
         <v>1</v>
@@ -2524,7 +2524,7 @@
         <v>-1</v>
       </c>
       <c r="F68" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G68" t="n">
         <v>9</v>
@@ -2555,7 +2555,7 @@
         <v>1.5</v>
       </c>
       <c r="F69" t="n">
-        <v>4.25</v>
+        <v>1</v>
       </c>
       <c r="G69" t="n">
         <v>1.25</v>
@@ -2586,7 +2586,7 @@
         <v>5</v>
       </c>
       <c r="F70" t="n">
-        <v>5.333333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G70" t="n">
         <v>1.333333333333333</v>
@@ -2617,7 +2617,7 @@
         <v>4.6</v>
       </c>
       <c r="F71" t="n">
-        <v>6.6</v>
+        <v>1.4</v>
       </c>
       <c r="G71" t="n">
         <v>2</v>
@@ -2648,7 +2648,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="F72" t="n">
-        <v>3.857142857142857</v>
+        <v>1</v>
       </c>
       <c r="G72" t="n">
         <v>1</v>
@@ -2679,7 +2679,7 @@
         <v>1.5</v>
       </c>
       <c r="F73" t="n">
-        <v>4.0625</v>
+        <v>0.625</v>
       </c>
       <c r="G73" t="n">
         <v>1.1875</v>
@@ -2710,7 +2710,7 @@
         <v>-4</v>
       </c>
       <c r="F74" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G74" t="n">
         <v>1</v>
@@ -2741,7 +2741,7 @@
         <v>2.5</v>
       </c>
       <c r="F75" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G75" t="n">
         <v>1.5</v>
@@ -2772,7 +2772,7 @@
         <v>0.5</v>
       </c>
       <c r="F76" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G76" t="n">
         <v>2</v>
@@ -2803,7 +2803,7 @@
         <v>3.5</v>
       </c>
       <c r="F77" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G77" t="n">
         <v>9</v>
@@ -2834,7 +2834,7 @@
         <v>-3</v>
       </c>
       <c r="F78" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G78" t="n">
         <v>3</v>
@@ -2865,7 +2865,7 @@
         <v>0.2</v>
       </c>
       <c r="F79" t="n">
-        <v>5.333333333333333</v>
+        <v>1.6</v>
       </c>
       <c r="G79" t="n">
         <v>1.2</v>
@@ -2896,7 +2896,7 @@
         <v>1.652173913043478</v>
       </c>
       <c r="F80" t="n">
-        <v>4.739130434782608</v>
+        <v>1.173913043478261</v>
       </c>
       <c r="G80" t="n">
         <v>1</v>
@@ -2927,7 +2927,7 @@
         <v>-1.285714285714286</v>
       </c>
       <c r="F81" t="n">
-        <v>5.857142857142857</v>
+        <v>1</v>
       </c>
       <c r="G81" t="n">
         <v>1.285714285714286</v>
@@ -2958,7 +2958,7 @@
         <v>-1</v>
       </c>
       <c r="F82" t="n">
-        <v>6.555555555555555</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="G82" t="n">
         <v>1.444444444444444</v>
@@ -2989,7 +2989,7 @@
         <v>3.5</v>
       </c>
       <c r="F83" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="G83" t="n">
         <v>2.5</v>
@@ -3020,7 +3020,7 @@
         <v>-7</v>
       </c>
       <c r="F84" t="n">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="G84" t="n">
         <v>1</v>
@@ -3051,7 +3051,7 @@
         <v>3</v>
       </c>
       <c r="F85" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G85" t="n">
         <v>1</v>
@@ -3082,7 +3082,7 @@
         <v>-4</v>
       </c>
       <c r="F86" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G86" t="n">
         <v>3</v>
@@ -3113,7 +3113,7 @@
         <v>1.802816901408451</v>
       </c>
       <c r="F87" t="n">
-        <v>4.450704225352113</v>
+        <v>1</v>
       </c>
       <c r="G87" t="n">
         <v>1.042253521126761</v>
@@ -3144,7 +3144,7 @@
         <v>-1.444444444444444</v>
       </c>
       <c r="F88" t="n">
-        <v>5</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="G88" t="n">
         <v>1.111111111111111</v>
@@ -3175,7 +3175,7 @@
         <v>-11</v>
       </c>
       <c r="F89" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G89" t="n">
         <v>1</v>
@@ -3206,7 +3206,7 @@
         <v>-13</v>
       </c>
       <c r="F90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G90" t="n">
         <v>1</v>
@@ -3237,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G91" t="n">
         <v>9</v>
@@ -3268,7 +3268,7 @@
         <v>8</v>
       </c>
       <c r="F92" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G92" t="n">
         <v>1</v>
@@ -3299,7 +3299,7 @@
         <v>-2.25</v>
       </c>
       <c r="F93" t="n">
-        <v>3.9375</v>
+        <v>1</v>
       </c>
       <c r="G93" t="n">
         <v>1.125</v>
@@ -3330,7 +3330,7 @@
         <v>2</v>
       </c>
       <c r="F94" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G94" t="n">
         <v>5</v>
@@ -3361,7 +3361,7 @@
         <v>-0.6666666666666666</v>
       </c>
       <c r="F95" t="n">
-        <v>3.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G95" t="n">
         <v>1</v>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>4</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G96" t="n">
         <v>1.333333333333333</v>
@@ -3423,7 +3423,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F97" t="n">
-        <v>4.5</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G97" t="n">
         <v>1</v>
@@ -3454,7 +3454,7 @@
         <v>-11</v>
       </c>
       <c r="F98" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G98" t="n">
         <v>2</v>
@@ -3485,7 +3485,7 @@
         <v>8</v>
       </c>
       <c r="F99" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G99" t="n">
         <v>1</v>
@@ -3516,7 +3516,7 @@
         <v>-5</v>
       </c>
       <c r="F100" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="G100" t="n">
         <v>2</v>
@@ -3547,7 +3547,7 @@
         <v>-1.5</v>
       </c>
       <c r="F101" t="n">
-        <v>5.25</v>
+        <v>1</v>
       </c>
       <c r="G101" t="n">
         <v>1.25</v>
@@ -3578,7 +3578,7 @@
         <v>-2.2</v>
       </c>
       <c r="F102" t="n">
-        <v>4.6</v>
+        <v>1.2</v>
       </c>
       <c r="G102" t="n">
         <v>1.2</v>
@@ -3609,7 +3609,7 @@
         <v>0.5</v>
       </c>
       <c r="F103" t="n">
-        <v>4.25</v>
+        <v>1</v>
       </c>
       <c r="G103" t="n">
         <v>1.25</v>
@@ -3640,7 +3640,7 @@
         <v>-2.25</v>
       </c>
       <c r="F104" t="n">
-        <v>4.25</v>
+        <v>1.25</v>
       </c>
       <c r="G104" t="n">
         <v>1.25</v>
@@ -3671,7 +3671,7 @@
         <v>6</v>
       </c>
       <c r="F105" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G105" t="n">
         <v>1</v>
@@ -3702,7 +3702,7 @@
         <v>-3</v>
       </c>
       <c r="F106" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G106" t="n">
         <v>3</v>
@@ -3733,7 +3733,7 @@
         <v>-1</v>
       </c>
       <c r="F107" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="G107" t="n">
         <v>1</v>
@@ -3764,7 +3764,7 @@
         <v>-1</v>
       </c>
       <c r="F108" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G108" t="n">
         <v>1.5</v>
@@ -3795,7 +3795,7 @@
         <v>-3</v>
       </c>
       <c r="F109" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G109" t="n">
         <v>2</v>
@@ -3826,7 +3826,7 @@
         <v>-6</v>
       </c>
       <c r="F110" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G110" t="n">
         <v>4</v>
@@ -3857,7 +3857,7 @@
         <v>3</v>
       </c>
       <c r="F111" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G111" t="n">
         <v>1</v>
@@ -3888,7 +3888,7 @@
         <v>0.6875</v>
       </c>
       <c r="F112" t="n">
-        <v>5.1875</v>
+        <v>1</v>
       </c>
       <c r="G112" t="n">
         <v>1.375</v>
@@ -3919,7 +3919,7 @@
         <v>1.5</v>
       </c>
       <c r="F113" t="n">
-        <v>4.75</v>
+        <v>1</v>
       </c>
       <c r="G113" t="n">
         <v>1.25</v>
@@ -3950,7 +3950,7 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="F114" t="n">
-        <v>4.333333333333333</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="G114" t="n">
         <v>1</v>
@@ -3981,7 +3981,7 @@
         <v>-3</v>
       </c>
       <c r="F115" t="n">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="G115" t="n">
         <v>2.5</v>
@@ -4012,7 +4012,7 @@
         <v>-2</v>
       </c>
       <c r="F116" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G116" t="n">
         <v>3</v>
@@ -4043,7 +4043,7 @@
         <v>2.416666666666667</v>
       </c>
       <c r="F117" t="n">
-        <v>4.5</v>
+        <v>1.083333333333333</v>
       </c>
       <c r="G117" t="n">
         <v>1.166666666666667</v>
@@ -4074,7 +4074,7 @@
         <v>1.829787234042553</v>
       </c>
       <c r="F118" t="n">
-        <v>5.936170212765957</v>
+        <v>1.25531914893617</v>
       </c>
       <c r="G118" t="n">
         <v>1.042553191489362</v>
@@ -4105,7 +4105,7 @@
         <v>1.875</v>
       </c>
       <c r="F119" t="n">
-        <v>8.5</v>
+        <v>1.625</v>
       </c>
       <c r="G119" t="n">
         <v>1.75</v>
@@ -4136,7 +4136,7 @@
         <v>4</v>
       </c>
       <c r="F120" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G120" t="n">
         <v>1</v>
@@ -4167,7 +4167,7 @@
         <v>-5.5</v>
       </c>
       <c r="F121" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G121" t="n">
         <v>3.5</v>
@@ -4198,7 +4198,7 @@
         <v>1.45</v>
       </c>
       <c r="F122" t="n">
-        <v>5.1</v>
+        <v>1.175</v>
       </c>
       <c r="G122" t="n">
         <v>1.05</v>
@@ -4229,7 +4229,7 @@
         <v>1.469387755102041</v>
       </c>
       <c r="F123" t="n">
-        <v>4.408163265306122</v>
+        <v>0.8775510204081632</v>
       </c>
       <c r="G123" t="n">
         <v>1.020408163265306</v>
@@ -4260,7 +4260,7 @@
         <v>1.415094339622641</v>
       </c>
       <c r="F124" t="n">
-        <v>5.867924528301887</v>
+        <v>1.60377358490566</v>
       </c>
       <c r="G124" t="n">
         <v>1.132075471698113</v>
@@ -4291,7 +4291,7 @@
         <v>7.666666666666667</v>
       </c>
       <c r="F125" t="n">
-        <v>7.666666666666667</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="G125" t="n">
         <v>1.333333333333333</v>
@@ -4322,7 +4322,7 @@
         <v>7</v>
       </c>
       <c r="F126" t="n">
-        <v>7</v>
+        <v>2.5</v>
       </c>
       <c r="G126" t="n">
         <v>2</v>
@@ -4353,7 +4353,7 @@
         <v>-2</v>
       </c>
       <c r="F127" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G127" t="n">
         <v>2</v>
@@ -4384,7 +4384,7 @@
         <v>-7</v>
       </c>
       <c r="F128" t="n">
-        <v>9.666666666666666</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G128" t="n">
         <v>2.333333333333333</v>
@@ -4415,7 +4415,7 @@
         <v>2</v>
       </c>
       <c r="F129" t="n">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="G129" t="n">
         <v>1.333333333333333</v>
@@ -4446,7 +4446,7 @@
         <v>2.222222222222222</v>
       </c>
       <c r="F130" t="n">
-        <v>5.666666666666667</v>
+        <v>1.277777777777778</v>
       </c>
       <c r="G130" t="n">
         <v>1.277777777777778</v>
@@ -4477,7 +4477,7 @@
         <v>6</v>
       </c>
       <c r="F131" t="n">
-        <v>21</v>
+        <v>4.5</v>
       </c>
       <c r="G131" t="n">
         <v>6</v>
@@ -4508,7 +4508,7 @@
         <v>1.142857142857143</v>
       </c>
       <c r="F132" t="n">
-        <v>5.571428571428571</v>
+        <v>1.857142857142857</v>
       </c>
       <c r="G132" t="n">
         <v>1.142857142857143</v>
@@ -4539,7 +4539,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F133" t="n">
-        <v>4.431372549019608</v>
+        <v>0.8431372549019608</v>
       </c>
       <c r="G133" t="n">
         <v>1.019607843137255</v>
@@ -4570,7 +4570,7 @@
         <v>0.5</v>
       </c>
       <c r="F134" t="n">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="G134" t="n">
         <v>1.5</v>
@@ -4601,7 +4601,7 @@
         <v>0.9761904761904762</v>
       </c>
       <c r="F135" t="n">
-        <v>4.547619047619047</v>
+        <v>0.9523809523809523</v>
       </c>
       <c r="G135" t="n">
         <v>1</v>
@@ -4632,7 +4632,7 @@
         <v>0.3529411764705883</v>
       </c>
       <c r="F136" t="n">
-        <v>5.176470588235294</v>
+        <v>0.7647058823529411</v>
       </c>
       <c r="G136" t="n">
         <v>1.235294117647059</v>
@@ -4663,7 +4663,7 @@
         <v>-11.33333333333333</v>
       </c>
       <c r="F137" t="n">
-        <v>1.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="G137" t="n">
         <v>1.333333333333333</v>
@@ -4694,7 +4694,7 @@
         <v>0.5882352941176471</v>
       </c>
       <c r="F138" t="n">
-        <v>5.647058823529412</v>
+        <v>1.411764705882353</v>
       </c>
       <c r="G138" t="n">
         <v>1.058823529411765</v>
@@ -4725,7 +4725,7 @@
         <v>3</v>
       </c>
       <c r="F139" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G139" t="n">
         <v>9</v>
@@ -4756,7 +4756,7 @@
         <v>5</v>
       </c>
       <c r="F140" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G140" t="n">
         <v>9</v>
@@ -4787,7 +4787,7 @@
         <v>1.454545454545455</v>
       </c>
       <c r="F141" t="n">
-        <v>5</v>
+        <v>1.090909090909091</v>
       </c>
       <c r="G141" t="n">
         <v>1.181818181818182</v>
@@ -4818,7 +4818,7 @@
         <v>-0.1428571428571428</v>
       </c>
       <c r="F142" t="n">
-        <v>5.142857142857143</v>
+        <v>1</v>
       </c>
       <c r="G142" t="n">
         <v>1.285714285714286</v>
@@ -4849,7 +4849,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="F143" t="n">
-        <v>6</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G143" t="n">
         <v>1.666666666666667</v>
@@ -4880,7 +4880,7 @@
         <v>1.625</v>
       </c>
       <c r="F144" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G144" t="n">
         <v>1.25</v>
@@ -4911,7 +4911,7 @@
         <v>1.839285714285714</v>
       </c>
       <c r="F145" t="n">
-        <v>4.803571428571429</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="G145" t="n">
         <v>1.089285714285714</v>
@@ -4942,7 +4942,7 @@
         <v>-16</v>
       </c>
       <c r="F146" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G146" t="n">
         <v>1</v>
@@ -4973,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>6.6</v>
+        <v>1</v>
       </c>
       <c r="G147" t="n">
         <v>2</v>
@@ -5004,7 +5004,7 @@
         <v>4.2</v>
       </c>
       <c r="F148" t="n">
-        <v>5.5</v>
+        <v>1.6</v>
       </c>
       <c r="G148" t="n">
         <v>1.3</v>
@@ -5035,7 +5035,7 @@
         <v>1.282608695652174</v>
       </c>
       <c r="F149" t="n">
-        <v>3.826086956521739</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="G149" t="n">
         <v>1.130434782608696</v>
@@ -5066,7 +5066,7 @@
         <v>-2</v>
       </c>
       <c r="F150" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G150" t="n">
         <v>1</v>
@@ -5097,7 +5097,7 @@
         <v>-1.75</v>
       </c>
       <c r="F151" t="n">
-        <v>11.25</v>
+        <v>2.25</v>
       </c>
       <c r="G151" t="n">
         <v>3.125</v>
@@ -5128,7 +5128,7 @@
         <v>5</v>
       </c>
       <c r="F152" t="n">
-        <v>32.66666666666666</v>
+        <v>8</v>
       </c>
       <c r="G152" t="n">
         <v>9</v>
@@ -5159,7 +5159,7 @@
         <v>4.166666666666667</v>
       </c>
       <c r="F153" t="n">
-        <v>3.166666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G153" t="n">
         <v>1</v>
@@ -5190,7 +5190,7 @@
         <v>-1.363636363636364</v>
       </c>
       <c r="F154" t="n">
-        <v>5.454545454545454</v>
+        <v>1.272727272727273</v>
       </c>
       <c r="G154" t="n">
         <v>1.363636363636364</v>
@@ -5221,7 +5221,7 @@
         <v>-2.5</v>
       </c>
       <c r="F155" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G155" t="n">
         <v>1.5</v>
@@ -5252,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="F156" t="n">
-        <v>5.25</v>
+        <v>0.5</v>
       </c>
       <c r="G156" t="n">
         <v>1.25</v>
@@ -5283,7 +5283,7 @@
         <v>-3.333333333333333</v>
       </c>
       <c r="F157" t="n">
-        <v>4</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G157" t="n">
         <v>1</v>
@@ -5314,7 +5314,7 @@
         <v>-0.8</v>
       </c>
       <c r="F158" t="n">
-        <v>5</v>
+        <v>1.6</v>
       </c>
       <c r="G158" t="n">
         <v>1</v>
@@ -5345,7 +5345,7 @@
         <v>0.5</v>
       </c>
       <c r="F159" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G159" t="n">
         <v>2</v>
@@ -5376,7 +5376,7 @@
         <v>0.75</v>
       </c>
       <c r="F160" t="n">
-        <v>6.083333333333333</v>
+        <v>1.916666666666667</v>
       </c>
       <c r="G160" t="n">
         <v>1.166666666666667</v>
@@ -5407,7 +5407,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="F161" t="n">
-        <v>4.416666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G161" t="n">
         <v>1.333333333333333</v>
@@ -5438,7 +5438,7 @@
         <v>-2</v>
       </c>
       <c r="F162" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G162" t="n">
         <v>1</v>
@@ -5469,7 +5469,7 @@
         <v>2.461538461538462</v>
       </c>
       <c r="F163" t="n">
-        <v>6.846153846153846</v>
+        <v>1.692307692307692</v>
       </c>
       <c r="G163" t="n">
         <v>1.538461538461539</v>
@@ -5500,7 +5500,7 @@
         <v>3</v>
       </c>
       <c r="F164" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="G164" t="n">
         <v>9</v>
@@ -5531,7 +5531,7 @@
         <v>5.5</v>
       </c>
       <c r="F165" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="G165" t="n">
         <v>9</v>
@@ -5562,7 +5562,7 @@
         <v>5</v>
       </c>
       <c r="F166" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G166" t="n">
         <v>1</v>
@@ -5593,7 +5593,7 @@
         <v>-7</v>
       </c>
       <c r="F167" t="n">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="G167" t="n">
         <v>1.5</v>
@@ -5624,7 +5624,7 @@
         <v>-3.2</v>
       </c>
       <c r="F168" t="n">
-        <v>3.2</v>
+        <v>1</v>
       </c>
       <c r="G168" t="n">
         <v>1.2</v>
@@ -5655,7 +5655,7 @@
         <v>0.8947368421052632</v>
       </c>
       <c r="F169" t="n">
-        <v>5.105263157894737</v>
+        <v>1.105263157894737</v>
       </c>
       <c r="G169" t="n">
         <v>1.105263157894737</v>
@@ -5686,7 +5686,7 @@
         <v>3.428571428571428</v>
       </c>
       <c r="F170" t="n">
-        <v>3.571428571428572</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G170" t="n">
         <v>1</v>
@@ -5717,7 +5717,7 @@
         <v>-4.5</v>
       </c>
       <c r="F171" t="n">
-        <v>8.5</v>
+        <v>1</v>
       </c>
       <c r="G171" t="n">
         <v>2</v>
@@ -5748,7 +5748,7 @@
         <v>2</v>
       </c>
       <c r="F172" t="n">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="G172" t="n">
         <v>1</v>
@@ -5779,7 +5779,7 @@
         <v>-6</v>
       </c>
       <c r="F173" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="G173" t="n">
         <v>1.5</v>
@@ -5810,7 +5810,7 @@
         <v>1.297297297297297</v>
       </c>
       <c r="F174" t="n">
-        <v>4.27027027027027</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="G174" t="n">
         <v>1.216216216216216</v>
@@ -5841,7 +5841,7 @@
         <v>-0.75</v>
       </c>
       <c r="F175" t="n">
-        <v>6.5</v>
+        <v>2.25</v>
       </c>
       <c r="G175" t="n">
         <v>1.75</v>
@@ -5872,7 +5872,7 @@
         <v>-1.857142857142857</v>
       </c>
       <c r="F176" t="n">
-        <v>5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G176" t="n">
         <v>1.428571428571429</v>
@@ -5903,7 +5903,7 @@
         <v>-12</v>
       </c>
       <c r="F177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G177" t="n">
         <v>1</v>
@@ -5934,7 +5934,7 @@
         <v>0.5</v>
       </c>
       <c r="F178" t="n">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="G178" t="n">
         <v>2.5</v>
@@ -5965,7 +5965,7 @@
         <v>0.25</v>
       </c>
       <c r="F179" t="n">
-        <v>11.25</v>
+        <v>2.25</v>
       </c>
       <c r="G179" t="n">
         <v>2.75</v>
@@ -5996,7 +5996,7 @@
         <v>1.132352941176471</v>
       </c>
       <c r="F180" t="n">
-        <v>5.382352941176471</v>
+        <v>1.294117647058824</v>
       </c>
       <c r="G180" t="n">
         <v>1.073529411764706</v>
@@ -6027,7 +6027,7 @@
         <v>-5</v>
       </c>
       <c r="F181" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G181" t="n">
         <v>2</v>
@@ -6058,7 +6058,7 @@
         <v>3.5</v>
       </c>
       <c r="F182" t="n">
-        <v>5.166666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G182" t="n">
         <v>1.5</v>
@@ -6089,7 +6089,7 @@
         <v>-8</v>
       </c>
       <c r="F183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G183" t="n">
         <v>1</v>
@@ -6120,7 +6120,7 @@
         <v>3.25</v>
       </c>
       <c r="F184" t="n">
-        <v>7</v>
+        <v>1.25</v>
       </c>
       <c r="G184" t="n">
         <v>1.75</v>
@@ -6151,7 +6151,7 @@
         <v>-1.75</v>
       </c>
       <c r="F185" t="n">
-        <v>10.5</v>
+        <v>2</v>
       </c>
       <c r="G185" t="n">
         <v>2.25</v>
@@ -6182,7 +6182,7 @@
         <v>2</v>
       </c>
       <c r="F186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G186" t="n">
         <v>1</v>
@@ -6213,7 +6213,7 @@
         <v>5</v>
       </c>
       <c r="F187" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G187" t="n">
         <v>1</v>
@@ -6244,7 +6244,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="F188" t="n">
-        <v>6.5</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G188" t="n">
         <v>1.5</v>
@@ -6275,7 +6275,7 @@
         <v>2.25</v>
       </c>
       <c r="F189" t="n">
-        <v>5.5</v>
+        <v>0.75</v>
       </c>
       <c r="G189" t="n">
         <v>1.5</v>
@@ -6306,7 +6306,7 @@
         <v>-10</v>
       </c>
       <c r="F190" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G190" t="n">
         <v>1</v>
@@ -6337,7 +6337,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="F191" t="n">
-        <v>5.05</v>
+        <v>1.183333333333333</v>
       </c>
       <c r="G191" t="n">
         <v>1</v>
@@ -6368,7 +6368,7 @@
         <v>-3</v>
       </c>
       <c r="F192" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G192" t="n">
         <v>2.5</v>
@@ -6399,7 +6399,7 @@
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>6.333333333333333</v>
+        <v>1.5</v>
       </c>
       <c r="G193" t="n">
         <v>1.333333333333333</v>
@@ -6430,7 +6430,7 @@
         <v>-7</v>
       </c>
       <c r="F194" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G194" t="n">
         <v>4</v>
@@ -6461,7 +6461,7 @@
         <v>-15</v>
       </c>
       <c r="F195" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G195" t="n">
         <v>2</v>
@@ -6492,7 +6492,7 @@
         <v>6.333333333333333</v>
       </c>
       <c r="F196" t="n">
-        <v>2.666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G196" t="n">
         <v>1</v>
@@ -6523,7 +6523,7 @@
         <v>2</v>
       </c>
       <c r="F197" t="n">
-        <v>7.5</v>
+        <v>0.75</v>
       </c>
       <c r="G197" t="n">
         <v>2</v>
@@ -6554,7 +6554,7 @@
         <v>4</v>
       </c>
       <c r="F198" t="n">
-        <v>7.8</v>
+        <v>2.2</v>
       </c>
       <c r="G198" t="n">
         <v>1.8</v>
@@ -6585,7 +6585,7 @@
         <v>-0.5</v>
       </c>
       <c r="F199" t="n">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="G199" t="n">
         <v>1.5</v>
@@ -6616,7 +6616,7 @@
         <v>3</v>
       </c>
       <c r="F200" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G200" t="n">
         <v>1</v>
@@ -6647,7 +6647,7 @@
         <v>5.5</v>
       </c>
       <c r="F201" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G201" t="n">
         <v>1</v>
@@ -6678,7 +6678,7 @@
         <v>3.625</v>
       </c>
       <c r="F202" t="n">
-        <v>5.125</v>
+        <v>1.25</v>
       </c>
       <c r="G202" t="n">
         <v>1</v>
@@ -6709,7 +6709,7 @@
         <v>1.857142857142857</v>
       </c>
       <c r="F203" t="n">
-        <v>4.571428571428571</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G203" t="n">
         <v>1.285714285714286</v>
@@ -6740,7 +6740,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="G204" t="n">
         <v>2</v>
@@ -6771,7 +6771,7 @@
         <v>10</v>
       </c>
       <c r="F205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G205" t="n">
         <v>1</v>
@@ -6802,7 +6802,7 @@
         <v>2.8</v>
       </c>
       <c r="F206" t="n">
-        <v>4.2</v>
+        <v>1</v>
       </c>
       <c r="G206" t="n">
         <v>1.2</v>
@@ -6833,7 +6833,7 @@
         <v>-11</v>
       </c>
       <c r="F207" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G207" t="n">
         <v>1</v>
@@ -6864,7 +6864,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="F208" t="n">
-        <v>4</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G208" t="n">
         <v>1</v>
@@ -6895,7 +6895,7 @@
         <v>0.1</v>
       </c>
       <c r="F209" t="n">
-        <v>3.9</v>
+        <v>0.7</v>
       </c>
       <c r="G209" t="n">
         <v>1.1</v>
@@ -6926,7 +6926,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="F210" t="n">
-        <v>5.857142857142857</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G210" t="n">
         <v>1.285714285714286</v>
@@ -6957,7 +6957,7 @@
         <v>1</v>
       </c>
       <c r="F211" t="n">
-        <v>7.6</v>
+        <v>1.6</v>
       </c>
       <c r="G211" t="n">
         <v>2.2</v>
@@ -6988,7 +6988,7 @@
         <v>1.88</v>
       </c>
       <c r="F212" t="n">
-        <v>4.32</v>
+        <v>1.16</v>
       </c>
       <c r="G212" t="n">
         <v>1.04</v>
@@ -7019,7 +7019,7 @@
         <v>-0.75</v>
       </c>
       <c r="F213" t="n">
-        <v>8.25</v>
+        <v>2</v>
       </c>
       <c r="G213" t="n">
         <v>1.25</v>
@@ -7050,7 +7050,7 @@
         <v>2</v>
       </c>
       <c r="F214" t="n">
-        <v>6.333333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G214" t="n">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>1.64</v>
       </c>
       <c r="F215" t="n">
-        <v>5.74</v>
+        <v>1.06</v>
       </c>
       <c r="G215" t="n">
         <v>1.1</v>
@@ -7112,7 +7112,7 @@
         <v>1.857142857142857</v>
       </c>
       <c r="F216" t="n">
-        <v>5.047619047619047</v>
+        <v>1.095238095238095</v>
       </c>
       <c r="G216" t="n">
         <v>1.428571428571429</v>
@@ -7143,7 +7143,7 @@
         <v>2.272727272727273</v>
       </c>
       <c r="F217" t="n">
-        <v>5.727272727272728</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G217" t="n">
         <v>1.636363636363636</v>
@@ -7174,7 +7174,7 @@
         <v>2</v>
       </c>
       <c r="F218" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="G218" t="n">
         <v>9</v>
@@ -7205,7 +7205,7 @@
         <v>2.8</v>
       </c>
       <c r="F219" t="n">
-        <v>9.4</v>
+        <v>1.4</v>
       </c>
       <c r="G219" t="n">
         <v>2.4</v>
@@ -7236,7 +7236,7 @@
         <v>-4.5</v>
       </c>
       <c r="F220" t="n">
-        <v>19.5</v>
+        <v>5</v>
       </c>
       <c r="G220" t="n">
         <v>3.5</v>
@@ -7267,7 +7267,7 @@
         <v>2.315789473684211</v>
       </c>
       <c r="F221" t="n">
-        <v>4.684210526315789</v>
+        <v>1.052631578947368</v>
       </c>
       <c r="G221" t="n">
         <v>1</v>
@@ -7298,7 +7298,7 @@
         <v>0</v>
       </c>
       <c r="F222" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G222" t="n">
         <v>1</v>
@@ -7329,7 +7329,7 @@
         <v>-3.2</v>
       </c>
       <c r="F223" t="n">
-        <v>7</v>
+        <v>0.6</v>
       </c>
       <c r="G223" t="n">
         <v>1.6</v>
@@ -7360,7 +7360,7 @@
         <v>5</v>
       </c>
       <c r="F224" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G224" t="n">
         <v>1</v>
@@ -7379,25 +7379,25 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.9259259259259259</v>
+        <v>1.018181818181818</v>
       </c>
       <c r="C225" t="n">
-        <v>13.83333333333333</v>
+        <v>13.94545454545455</v>
       </c>
       <c r="D225" t="n">
-        <v>2.296296296296296</v>
+        <v>2.309090909090909</v>
       </c>
       <c r="E225" t="n">
-        <v>2.055555555555555</v>
+        <v>2</v>
       </c>
       <c r="F225" t="n">
-        <v>4.611111111111111</v>
+        <v>1.036363636363636</v>
       </c>
       <c r="G225" t="n">
-        <v>1.037037037037037</v>
+        <v>1.054545454545454</v>
       </c>
       <c r="H225" t="n">
-        <v>8.962962962962964</v>
+        <v>8.945454545454545</v>
       </c>
       <c r="I225" t="n">
         <v>9</v>
@@ -7422,7 +7422,7 @@
         <v>-0.3333333333333333</v>
       </c>
       <c r="F226" t="n">
-        <v>9.333333333333334</v>
+        <v>1</v>
       </c>
       <c r="G226" t="n">
         <v>2.666666666666667</v>
@@ -7453,7 +7453,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="F227" t="n">
-        <v>7.428571428571429</v>
+        <v>2.142857142857143</v>
       </c>
       <c r="G227" t="n">
         <v>1.571428571428571</v>
@@ -7484,7 +7484,7 @@
         <v>-0.3</v>
       </c>
       <c r="F228" t="n">
-        <v>5.8</v>
+        <v>1.2</v>
       </c>
       <c r="G228" t="n">
         <v>1.4</v>
@@ -7515,7 +7515,7 @@
         <v>4</v>
       </c>
       <c r="F229" t="n">
-        <v>6</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G229" t="n">
         <v>1.333333333333333</v>
@@ -7546,7 +7546,7 @@
         <v>1.38</v>
       </c>
       <c r="F230" t="n">
-        <v>4.76</v>
+        <v>1.16</v>
       </c>
       <c r="G230" t="n">
         <v>1.1</v>
@@ -7577,7 +7577,7 @@
         <v>2.615384615384615</v>
       </c>
       <c r="F231" t="n">
-        <v>5.076923076923077</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="G231" t="n">
         <v>1.461538461538461</v>
@@ -7608,7 +7608,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F232" t="n">
-        <v>5</v>
+        <v>1.266666666666667</v>
       </c>
       <c r="G232" t="n">
         <v>1</v>
@@ -7639,7 +7639,7 @@
         <v>2.5</v>
       </c>
       <c r="F233" t="n">
-        <v>13.5</v>
+        <v>2</v>
       </c>
       <c r="G233" t="n">
         <v>2.5</v>
@@ -7670,7 +7670,7 @@
         <v>0.75</v>
       </c>
       <c r="F234" t="n">
-        <v>5.25</v>
+        <v>1.5</v>
       </c>
       <c r="G234" t="n">
         <v>1.25</v>
@@ -7701,7 +7701,7 @@
         <v>-1.6</v>
       </c>
       <c r="F235" t="n">
-        <v>6.2</v>
+        <v>1</v>
       </c>
       <c r="G235" t="n">
         <v>1</v>
@@ -7732,7 +7732,7 @@
         <v>0.8</v>
       </c>
       <c r="F236" t="n">
-        <v>4</v>
+        <v>0.6</v>
       </c>
       <c r="G236" t="n">
         <v>1</v>
@@ -7763,7 +7763,7 @@
         <v>2.636363636363636</v>
       </c>
       <c r="F237" t="n">
-        <v>5.181818181818182</v>
+        <v>1.272727272727273</v>
       </c>
       <c r="G237" t="n">
         <v>1.272727272727273</v>
@@ -7794,7 +7794,7 @@
         <v>4.666666666666667</v>
       </c>
       <c r="F238" t="n">
-        <v>10.66666666666667</v>
+        <v>2</v>
       </c>
       <c r="G238" t="n">
         <v>2.333333333333333</v>
@@ -7825,7 +7825,7 @@
         <v>-1.5</v>
       </c>
       <c r="F239" t="n">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="G239" t="n">
         <v>2.5</v>
@@ -7856,7 +7856,7 @@
         <v>-2</v>
       </c>
       <c r="F240" t="n">
-        <v>3.625</v>
+        <v>0.5</v>
       </c>
       <c r="G240" t="n">
         <v>1.25</v>
@@ -7887,7 +7887,7 @@
         <v>3</v>
       </c>
       <c r="F241" t="n">
-        <v>7.8</v>
+        <v>1.6</v>
       </c>
       <c r="G241" t="n">
         <v>2.4</v>
@@ -7918,7 +7918,7 @@
         <v>3</v>
       </c>
       <c r="F242" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G242" t="n">
         <v>9</v>
@@ -7949,7 +7949,7 @@
         <v>-0.4444444444444444</v>
       </c>
       <c r="F243" t="n">
-        <v>5.111111111111111</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G243" t="n">
         <v>1.222222222222222</v>
@@ -7980,7 +7980,7 @@
         <v>-0.09090909090909091</v>
       </c>
       <c r="F244" t="n">
-        <v>4.454545454545454</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G244" t="n">
         <v>1</v>
@@ -8011,7 +8011,7 @@
         <v>1.142857142857143</v>
       </c>
       <c r="F245" t="n">
-        <v>7.714285714285714</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="G245" t="n">
         <v>1.571428571428571</v>
@@ -8042,7 +8042,7 @@
         <v>0</v>
       </c>
       <c r="F246" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G246" t="n">
         <v>1</v>
@@ -8073,7 +8073,7 @@
         <v>8</v>
       </c>
       <c r="F247" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G247" t="n">
         <v>3</v>
@@ -8104,7 +8104,7 @@
         <v>1.75</v>
       </c>
       <c r="F248" t="n">
-        <v>5.125</v>
+        <v>0.75</v>
       </c>
       <c r="G248" t="n">
         <v>1</v>
@@ -8135,7 +8135,7 @@
         <v>6</v>
       </c>
       <c r="F249" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G249" t="n">
         <v>1</v>
@@ -8166,7 +8166,7 @@
         <v>1.227272727272727</v>
       </c>
       <c r="F250" t="n">
-        <v>5.25</v>
+        <v>1.295454545454545</v>
       </c>
       <c r="G250" t="n">
         <v>1</v>
@@ -8228,7 +8228,7 @@
         <v>-1</v>
       </c>
       <c r="F252" t="n">
-        <v>3.4</v>
+        <v>0.7</v>
       </c>
       <c r="G252" t="n">
         <v>1.3</v>
@@ -8259,7 +8259,7 @@
         <v>0.55</v>
       </c>
       <c r="F253" t="n">
-        <v>5.3</v>
+        <v>1.1</v>
       </c>
       <c r="G253" t="n">
         <v>1</v>
@@ -8290,7 +8290,7 @@
         <v>-1</v>
       </c>
       <c r="F254" t="n">
-        <v>4.333333333333333</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G254" t="n">
         <v>1.166666666666667</v>
@@ -8321,7 +8321,7 @@
         <v>-12</v>
       </c>
       <c r="F255" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G255" t="n">
         <v>2</v>
@@ -8352,7 +8352,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="F256" t="n">
-        <v>4</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G256" t="n">
         <v>1.333333333333333</v>
@@ -8383,7 +8383,7 @@
         <v>0.3</v>
       </c>
       <c r="F257" t="n">
-        <v>4.4</v>
+        <v>0.5</v>
       </c>
       <c r="G257" t="n">
         <v>1.2</v>
@@ -8414,7 +8414,7 @@
         <v>0.7435897435897436</v>
       </c>
       <c r="F258" t="n">
-        <v>5.487179487179487</v>
+        <v>1.205128205128205</v>
       </c>
       <c r="G258" t="n">
         <v>1.102564102564103</v>
@@ -8445,7 +8445,7 @@
         <v>-1</v>
       </c>
       <c r="F259" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G259" t="n">
         <v>1</v>
@@ -8476,7 +8476,7 @@
         <v>-1</v>
       </c>
       <c r="F260" t="n">
-        <v>6.8</v>
+        <v>2.2</v>
       </c>
       <c r="G260" t="n">
         <v>1.6</v>
@@ -8507,7 +8507,7 @@
         <v>-5.666666666666667</v>
       </c>
       <c r="F261" t="n">
-        <v>7</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G261" t="n">
         <v>1.333333333333333</v>
@@ -8538,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="F262" t="n">
-        <v>3.888888888888889</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G262" t="n">
         <v>1.111111111111111</v>
@@ -8569,7 +8569,7 @@
         <v>6</v>
       </c>
       <c r="F263" t="n">
-        <v>8.666666666666666</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G263" t="n">
         <v>2.666666666666667</v>
@@ -8600,7 +8600,7 @@
         <v>3</v>
       </c>
       <c r="F264" t="n">
-        <v>4.666666666666667</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G264" t="n">
         <v>1.333333333333333</v>
@@ -8631,7 +8631,7 @@
         <v>1.4</v>
       </c>
       <c r="F265" t="n">
-        <v>4.4</v>
+        <v>0.8</v>
       </c>
       <c r="G265" t="n">
         <v>1.4</v>
@@ -8662,7 +8662,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F266" t="n">
-        <v>3.666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="G266" t="n">
         <v>1</v>
@@ -8693,7 +8693,7 @@
         <v>1.8</v>
       </c>
       <c r="F267" t="n">
-        <v>2.6</v>
+        <v>0.8</v>
       </c>
       <c r="G267" t="n">
         <v>1.2</v>
@@ -8724,7 +8724,7 @@
         <v>-2.476190476190476</v>
       </c>
       <c r="F268" t="n">
-        <v>5</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G268" t="n">
         <v>1.19047619047619</v>
@@ -8755,7 +8755,7 @@
         <v>1.076923076923077</v>
       </c>
       <c r="F269" t="n">
-        <v>4.538461538461538</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="G269" t="n">
         <v>1.384615384615385</v>
@@ -8786,7 +8786,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F270" t="n">
-        <v>2.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="G270" t="n">
         <v>1.666666666666667</v>
@@ -8817,7 +8817,7 @@
         <v>0.2307692307692308</v>
       </c>
       <c r="F271" t="n">
-        <v>5.384615384615385</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="G271" t="n">
         <v>1.384615384615385</v>
@@ -8848,7 +8848,7 @@
         <v>1.363636363636364</v>
       </c>
       <c r="F272" t="n">
-        <v>5.545454545454546</v>
+        <v>1.545454545454545</v>
       </c>
       <c r="G272" t="n">
         <v>1.090909090909091</v>
@@ -8879,7 +8879,7 @@
         <v>-5.75</v>
       </c>
       <c r="F273" t="n">
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
       <c r="G273" t="n">
         <v>2</v>
@@ -8910,7 +8910,7 @@
         <v>-12</v>
       </c>
       <c r="F274" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G274" t="n">
         <v>4</v>
@@ -8941,7 +8941,7 @@
         <v>-2</v>
       </c>
       <c r="F275" t="n">
-        <v>6.166666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="G275" t="n">
         <v>1</v>
@@ -8972,7 +8972,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="F276" t="n">
-        <v>4.333333333333333</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G276" t="n">
         <v>1</v>
@@ -9003,7 +9003,7 @@
         <v>-1.333333333333333</v>
       </c>
       <c r="F277" t="n">
-        <v>7.666666666666667</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="G277" t="n">
         <v>2</v>
@@ -9034,7 +9034,7 @@
         <v>0.625</v>
       </c>
       <c r="F278" t="n">
-        <v>4.75</v>
+        <v>0.875</v>
       </c>
       <c r="G278" t="n">
         <v>1.125</v>
@@ -9065,7 +9065,7 @@
         <v>-1.5</v>
       </c>
       <c r="F279" t="n">
-        <v>3.666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G279" t="n">
         <v>1.5</v>
@@ -9096,7 +9096,7 @@
         <v>-8</v>
       </c>
       <c r="F280" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G280" t="n">
         <v>1</v>
@@ -9127,7 +9127,7 @@
         <v>10.5</v>
       </c>
       <c r="F281" t="n">
-        <v>11.5</v>
+        <v>3.5</v>
       </c>
       <c r="G281" t="n">
         <v>2</v>
@@ -9158,7 +9158,7 @@
         <v>-1.2</v>
       </c>
       <c r="F282" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G282" t="n">
         <v>1.4</v>
@@ -9189,7 +9189,7 @@
         <v>-1</v>
       </c>
       <c r="F283" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G283" t="n">
         <v>1</v>
@@ -9220,7 +9220,7 @@
         <v>1.5</v>
       </c>
       <c r="F284" t="n">
-        <v>3.25</v>
+        <v>0.5</v>
       </c>
       <c r="G284" t="n">
         <v>1.25</v>
@@ -9251,7 +9251,7 @@
         <v>0</v>
       </c>
       <c r="F285" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G285" t="n">
         <v>1</v>
@@ -9282,7 +9282,7 @@
         <v>0.8</v>
       </c>
       <c r="F286" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G286" t="n">
         <v>1</v>
@@ -9313,7 +9313,7 @@
         <v>3</v>
       </c>
       <c r="F287" t="n">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="G287" t="n">
         <v>9</v>
@@ -9344,7 +9344,7 @@
         <v>10</v>
       </c>
       <c r="F288" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G288" t="n">
         <v>1</v>
@@ -9375,7 +9375,7 @@
         <v>1.5</v>
       </c>
       <c r="F289" t="n">
-        <v>8.5</v>
+        <v>1</v>
       </c>
       <c r="G289" t="n">
         <v>2</v>
@@ -9406,7 +9406,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="F290" t="n">
-        <v>5.416666666666667</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G290" t="n">
         <v>1.083333333333333</v>
@@ -9437,7 +9437,7 @@
         <v>8</v>
       </c>
       <c r="F291" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G291" t="n">
         <v>2</v>
@@ -9468,7 +9468,7 @@
         <v>-13</v>
       </c>
       <c r="F292" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G292" t="n">
         <v>1</v>
@@ -9499,7 +9499,7 @@
         <v>0.125</v>
       </c>
       <c r="F293" t="n">
-        <v>3.375</v>
+        <v>0.75</v>
       </c>
       <c r="G293" t="n">
         <v>1</v>
@@ -9530,7 +9530,7 @@
         <v>-1</v>
       </c>
       <c r="F294" t="n">
-        <v>5.5</v>
+        <v>1.75</v>
       </c>
       <c r="G294" t="n">
         <v>1</v>
@@ -9561,7 +9561,7 @@
         <v>6</v>
       </c>
       <c r="F295" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G295" t="n">
         <v>1</v>
@@ -9592,7 +9592,7 @@
         <v>-1.142857142857143</v>
       </c>
       <c r="F296" t="n">
-        <v>4.571428571428571</v>
+        <v>1.285714285714286</v>
       </c>
       <c r="G296" t="n">
         <v>1.285714285714286</v>
@@ -9623,7 +9623,7 @@
         <v>-0.75</v>
       </c>
       <c r="F297" t="n">
-        <v>3.75</v>
+        <v>1</v>
       </c>
       <c r="G297" t="n">
         <v>1</v>
@@ -9654,7 +9654,7 @@
         <v>1.625</v>
       </c>
       <c r="F298" t="n">
-        <v>4.75</v>
+        <v>1</v>
       </c>
       <c r="G298" t="n">
         <v>1</v>
@@ -9685,7 +9685,7 @@
         <v>2.347826086956522</v>
       </c>
       <c r="F299" t="n">
-        <v>4.782608695652174</v>
+        <v>1.217391304347826</v>
       </c>
       <c r="G299" t="n">
         <v>1.217391304347826</v>
@@ -9716,7 +9716,7 @@
         <v>2</v>
       </c>
       <c r="F300" t="n">
-        <v>6.875</v>
+        <v>0.75</v>
       </c>
       <c r="G300" t="n">
         <v>1.5</v>
@@ -9747,7 +9747,7 @@
         <v>-1.5</v>
       </c>
       <c r="F301" t="n">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="G301" t="n">
         <v>1.5</v>
@@ -9778,7 +9778,7 @@
         <v>-0.25</v>
       </c>
       <c r="F302" t="n">
-        <v>4.833333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="G302" t="n">
         <v>1.083333333333333</v>
@@ -9809,7 +9809,7 @@
         <v>0.5384615384615384</v>
       </c>
       <c r="F303" t="n">
-        <v>4.615384615384615</v>
+        <v>1</v>
       </c>
       <c r="G303" t="n">
         <v>1</v>
@@ -9840,7 +9840,7 @@
         <v>2</v>
       </c>
       <c r="F304" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G304" t="n">
         <v>1</v>
@@ -9871,7 +9871,7 @@
         <v>0.5</v>
       </c>
       <c r="F305" t="n">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="G305" t="n">
         <v>2</v>
@@ -9902,7 +9902,7 @@
         <v>5</v>
       </c>
       <c r="F306" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G306" t="n">
         <v>1</v>
@@ -9933,7 +9933,7 @@
         <v>1.846153846153846</v>
       </c>
       <c r="F307" t="n">
-        <v>4.538461538461538</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="G307" t="n">
         <v>1.153846153846154</v>
@@ -9964,7 +9964,7 @@
         <v>1.645161290322581</v>
       </c>
       <c r="F308" t="n">
-        <v>5.096774193548387</v>
+        <v>0.7741935483870968</v>
       </c>
       <c r="G308" t="n">
         <v>1.096774193548387</v>
@@ -9995,7 +9995,7 @@
         <v>0.5</v>
       </c>
       <c r="F309" t="n">
-        <v>15.5</v>
+        <v>3.5</v>
       </c>
       <c r="G309" t="n">
         <v>4</v>
@@ -10026,7 +10026,7 @@
         <v>0.75</v>
       </c>
       <c r="F310" t="n">
-        <v>5.5</v>
+        <v>0.625</v>
       </c>
       <c r="G310" t="n">
         <v>1.25</v>
@@ -10057,7 +10057,7 @@
         <v>-2.8</v>
       </c>
       <c r="F311" t="n">
-        <v>4.6</v>
+        <v>0.6</v>
       </c>
       <c r="G311" t="n">
         <v>1.2</v>
@@ -10088,7 +10088,7 @@
         <v>-10</v>
       </c>
       <c r="F312" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G312" t="n">
         <v>1</v>
@@ -10119,7 +10119,7 @@
         <v>-3.333333333333333</v>
       </c>
       <c r="F313" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G313" t="n">
         <v>1.333333333333333</v>
@@ -10150,7 +10150,7 @@
         <v>-1.153846153846154</v>
       </c>
       <c r="F314" t="n">
-        <v>6</v>
+        <v>1.153846153846154</v>
       </c>
       <c r="G314" t="n">
         <v>1.230769230769231</v>
@@ -10181,7 +10181,7 @@
         <v>-4</v>
       </c>
       <c r="F315" t="n">
-        <v>16</v>
+        <v>2.5</v>
       </c>
       <c r="G315" t="n">
         <v>2.5</v>
@@ -10212,7 +10212,7 @@
         <v>1.580645161290323</v>
       </c>
       <c r="F316" t="n">
-        <v>4.741935483870968</v>
+        <v>1.096774193548387</v>
       </c>
       <c r="G316" t="n">
         <v>1.096774193548387</v>
@@ -10243,7 +10243,7 @@
         <v>-12</v>
       </c>
       <c r="F317" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G317" t="n">
         <v>1</v>
@@ -10274,7 +10274,7 @@
         <v>3.666666666666667</v>
       </c>
       <c r="F318" t="n">
-        <v>4.333333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G318" t="n">
         <v>1</v>
@@ -10305,7 +10305,7 @@
         <v>3</v>
       </c>
       <c r="F319" t="n">
-        <v>6.5</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G319" t="n">
         <v>1.166666666666667</v>
@@ -10336,7 +10336,7 @@
         <v>-14</v>
       </c>
       <c r="F320" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G320" t="n">
         <v>2</v>
@@ -10367,7 +10367,7 @@
         <v>1.48936170212766</v>
       </c>
       <c r="F321" t="n">
-        <v>6.553191489361702</v>
+        <v>1.893617021276596</v>
       </c>
       <c r="G321" t="n">
         <v>1.191489361702128</v>
@@ -10398,7 +10398,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="F322" t="n">
-        <v>6.5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G322" t="n">
         <v>1.333333333333333</v>
@@ -10429,7 +10429,7 @@
         <v>1</v>
       </c>
       <c r="F323" t="n">
-        <v>4.5625</v>
+        <v>0.6875</v>
       </c>
       <c r="G323" t="n">
         <v>1.1875</v>
@@ -10460,7 +10460,7 @@
         <v>2.333333333333333</v>
       </c>
       <c r="F324" t="n">
-        <v>5.333333333333333</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G324" t="n">
         <v>1.5</v>
@@ -10491,7 +10491,7 @@
         <v>0.625</v>
       </c>
       <c r="F325" t="n">
-        <v>2.25</v>
+        <v>0.5</v>
       </c>
       <c r="G325" t="n">
         <v>1</v>
@@ -10522,7 +10522,7 @@
         <v>0.25</v>
       </c>
       <c r="F326" t="n">
-        <v>5.5</v>
+        <v>0.5</v>
       </c>
       <c r="G326" t="n">
         <v>1.25</v>
@@ -10553,7 +10553,7 @@
         <v>-1.2</v>
       </c>
       <c r="F327" t="n">
-        <v>3.8</v>
+        <v>0.8</v>
       </c>
       <c r="G327" t="n">
         <v>1</v>
@@ -10584,7 +10584,7 @@
         <v>-0.1111111111111111</v>
       </c>
       <c r="F328" t="n">
-        <v>6.111111111111111</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G328" t="n">
         <v>1.666666666666667</v>
@@ -10615,7 +10615,7 @@
         <v>4.833333333333333</v>
       </c>
       <c r="F329" t="n">
-        <v>5.833333333333333</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G329" t="n">
         <v>1</v>
@@ -10646,7 +10646,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="F330" t="n">
-        <v>2.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G330" t="n">
         <v>1</v>
@@ -10677,7 +10677,7 @@
         <v>2.5</v>
       </c>
       <c r="F331" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G331" t="n">
         <v>4</v>
@@ -10708,7 +10708,7 @@
         <v>-1</v>
       </c>
       <c r="F332" t="n">
-        <v>4.428571428571429</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="G332" t="n">
         <v>1.142857142857143</v>
@@ -10739,7 +10739,7 @@
         <v>1.142857142857143</v>
       </c>
       <c r="F333" t="n">
-        <v>6.285714285714286</v>
+        <v>2</v>
       </c>
       <c r="G333" t="n">
         <v>1.428571428571429</v>
@@ -10770,7 +10770,7 @@
         <v>-0.7777777777777778</v>
       </c>
       <c r="F334" t="n">
-        <v>3</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G334" t="n">
         <v>1.222222222222222</v>
@@ -10801,7 +10801,7 @@
         <v>3.5</v>
       </c>
       <c r="F335" t="n">
-        <v>7.5</v>
+        <v>1.75</v>
       </c>
       <c r="G335" t="n">
         <v>1.5</v>
@@ -10832,7 +10832,7 @@
         <v>2</v>
       </c>
       <c r="F336" t="n">
-        <v>5</v>
+        <v>1.25</v>
       </c>
       <c r="G336" t="n">
         <v>1.25</v>
@@ -10863,7 +10863,7 @@
         <v>1.723404255319149</v>
       </c>
       <c r="F337" t="n">
-        <v>5.595744680851064</v>
+        <v>1.297872340425532</v>
       </c>
       <c r="G337" t="n">
         <v>1.191489361702128</v>
@@ -10894,7 +10894,7 @@
         <v>1.25</v>
       </c>
       <c r="F338" t="n">
-        <v>5.375</v>
+        <v>0.75</v>
       </c>
       <c r="G338" t="n">
         <v>1.25</v>
@@ -10925,7 +10925,7 @@
         <v>0.25</v>
       </c>
       <c r="F339" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G339" t="n">
         <v>1.25</v>
@@ -10956,7 +10956,7 @@
         <v>5</v>
       </c>
       <c r="F340" t="n">
-        <v>8.333333333333334</v>
+        <v>2</v>
       </c>
       <c r="G340" t="n">
         <v>1.666666666666667</v>
@@ -10987,7 +10987,7 @@
         <v>-2.5</v>
       </c>
       <c r="F341" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G341" t="n">
         <v>1</v>
@@ -11018,7 +11018,7 @@
         <v>9</v>
       </c>
       <c r="F342" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G342" t="n">
         <v>3</v>
@@ -11049,7 +11049,7 @@
         <v>1.1</v>
       </c>
       <c r="F343" t="n">
-        <v>4.3</v>
+        <v>1.025</v>
       </c>
       <c r="G343" t="n">
         <v>1.025</v>
@@ -11080,7 +11080,7 @@
         <v>-8</v>
       </c>
       <c r="F344" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G344" t="n">
         <v>2</v>
@@ -11111,7 +11111,7 @@
         <v>-2.571428571428572</v>
       </c>
       <c r="F345" t="n">
-        <v>5.142857142857143</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G345" t="n">
         <v>1.142857142857143</v>
@@ -11142,7 +11142,7 @@
         <v>-3</v>
       </c>
       <c r="F346" t="n">
-        <v>8.5</v>
+        <v>2</v>
       </c>
       <c r="G346" t="n">
         <v>1.25</v>
@@ -11173,7 +11173,7 @@
         <v>4</v>
       </c>
       <c r="F347" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G347" t="n">
         <v>9</v>
@@ -11204,7 +11204,7 @@
         <v>-1.5</v>
       </c>
       <c r="F348" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G348" t="n">
         <v>1</v>
@@ -11235,7 +11235,7 @@
         <v>8</v>
       </c>
       <c r="F349" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="G349" t="n">
         <v>9</v>
@@ -11266,7 +11266,7 @@
         <v>1.444444444444444</v>
       </c>
       <c r="F350" t="n">
-        <v>5.444444444444445</v>
+        <v>1.222222222222222</v>
       </c>
       <c r="G350" t="n">
         <v>1.222222222222222</v>
@@ -11297,7 +11297,7 @@
         <v>0</v>
       </c>
       <c r="F351" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G351" t="n">
         <v>4</v>
@@ -11328,7 +11328,7 @@
         <v>3</v>
       </c>
       <c r="F352" t="n">
-        <v>4.4</v>
+        <v>1.2</v>
       </c>
       <c r="G352" t="n">
         <v>1.6</v>
@@ -11359,7 +11359,7 @@
         <v>5.666666666666667</v>
       </c>
       <c r="F353" t="n">
-        <v>12</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="G353" t="n">
         <v>3</v>
@@ -11390,7 +11390,7 @@
         <v>1.875</v>
       </c>
       <c r="F354" t="n">
-        <v>5.25</v>
+        <v>1.25</v>
       </c>
       <c r="G354" t="n">
         <v>1</v>
@@ -11421,7 +11421,7 @@
         <v>-2.166666666666667</v>
       </c>
       <c r="F355" t="n">
-        <v>5</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="G355" t="n">
         <v>1.5</v>
@@ -11452,7 +11452,7 @@
         <v>4.75</v>
       </c>
       <c r="F356" t="n">
-        <v>6.75</v>
+        <v>1.75</v>
       </c>
       <c r="G356" t="n">
         <v>1.5</v>
@@ -11483,7 +11483,7 @@
         <v>-5</v>
       </c>
       <c r="F357" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="G357" t="n">
         <v>2</v>
@@ -11514,7 +11514,7 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="F358" t="n">
-        <v>5.444444444444445</v>
+        <v>1</v>
       </c>
       <c r="G358" t="n">
         <v>1.555555555555556</v>
@@ -11545,7 +11545,7 @@
         <v>2</v>
       </c>
       <c r="F359" t="n">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="G359" t="n">
         <v>3</v>
@@ -11576,7 +11576,7 @@
         <v>1.8125</v>
       </c>
       <c r="F360" t="n">
-        <v>4.375</v>
+        <v>1.0625</v>
       </c>
       <c r="G360" t="n">
         <v>1</v>
@@ -11607,7 +11607,7 @@
         <v>-0.2142857142857143</v>
       </c>
       <c r="F361" t="n">
-        <v>5.071428571428571</v>
+        <v>1.285714285714286</v>
       </c>
       <c r="G361" t="n">
         <v>1.214285714285714</v>
@@ -11638,7 +11638,7 @@
         <v>1.25</v>
       </c>
       <c r="F362" t="n">
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="G362" t="n">
         <v>1</v>
@@ -11669,7 +11669,7 @@
         <v>-5.5</v>
       </c>
       <c r="F363" t="n">
-        <v>10.25</v>
+        <v>1</v>
       </c>
       <c r="G363" t="n">
         <v>2.25</v>
@@ -11700,7 +11700,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="F364" t="n">
-        <v>3.571428571428572</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G364" t="n">
         <v>1.285714285714286</v>
@@ -11731,7 +11731,7 @@
         <v>2</v>
       </c>
       <c r="F365" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G365" t="n">
         <v>1</v>
@@ -11762,7 +11762,7 @@
         <v>2.266666666666667</v>
       </c>
       <c r="F366" t="n">
-        <v>5.366666666666666</v>
+        <v>1.133333333333333</v>
       </c>
       <c r="G366" t="n">
         <v>1.033333333333333</v>
@@ -11793,7 +11793,7 @@
         <v>4</v>
       </c>
       <c r="F367" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G367" t="n">
         <v>1</v>
@@ -11824,7 +11824,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="F368" t="n">
-        <v>9.833333333333334</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G368" t="n">
         <v>2.166666666666667</v>
@@ -11855,7 +11855,7 @@
         <v>1.5</v>
       </c>
       <c r="F369" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G369" t="n">
         <v>1</v>
@@ -11886,7 +11886,7 @@
         <v>1</v>
       </c>
       <c r="F370" t="n">
-        <v>2.777777777777778</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G370" t="n">
         <v>1.222222222222222</v>
@@ -11917,7 +11917,7 @@
         <v>1</v>
       </c>
       <c r="F371" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G371" t="n">
         <v>2</v>
@@ -11948,7 +11948,7 @@
         <v>-9</v>
       </c>
       <c r="F372" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G372" t="n">
         <v>1</v>
@@ -11979,7 +11979,7 @@
         <v>2</v>
       </c>
       <c r="F373" t="n">
-        <v>5.428571428571429</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G373" t="n">
         <v>1.142857142857143</v>
@@ -12041,7 +12041,7 @@
         <v>2.25</v>
       </c>
       <c r="F375" t="n">
-        <v>5.375</v>
+        <v>1.125</v>
       </c>
       <c r="G375" t="n">
         <v>1.125</v>
@@ -12072,7 +12072,7 @@
         <v>1</v>
       </c>
       <c r="F376" t="n">
-        <v>5</v>
+        <v>1.25</v>
       </c>
       <c r="G376" t="n">
         <v>1.125</v>
@@ -12103,7 +12103,7 @@
         <v>1.25</v>
       </c>
       <c r="F377" t="n">
-        <v>6.25</v>
+        <v>1.25</v>
       </c>
       <c r="G377" t="n">
         <v>1</v>
@@ -12134,7 +12134,7 @@
         <v>-1</v>
       </c>
       <c r="F378" t="n">
-        <v>3.8</v>
+        <v>0.65</v>
       </c>
       <c r="G378" t="n">
         <v>1.05</v>
@@ -12165,7 +12165,7 @@
         <v>-3</v>
       </c>
       <c r="F379" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G379" t="n">
         <v>1</v>
@@ -12196,7 +12196,7 @@
         <v>-0.5714285714285714</v>
       </c>
       <c r="F380" t="n">
-        <v>6.428571428571429</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G380" t="n">
         <v>1.714285714285714</v>
@@ -12227,7 +12227,7 @@
         <v>-1.6</v>
       </c>
       <c r="F381" t="n">
-        <v>3.6</v>
+        <v>0.4</v>
       </c>
       <c r="G381" t="n">
         <v>1.2</v>
@@ -12258,7 +12258,7 @@
         <v>-0.8571428571428571</v>
       </c>
       <c r="F382" t="n">
-        <v>5.714285714285714</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G382" t="n">
         <v>1.571428571428571</v>
@@ -12289,7 +12289,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F383" t="n">
-        <v>10</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="G383" t="n">
         <v>2</v>
@@ -12320,7 +12320,7 @@
         <v>4</v>
       </c>
       <c r="F384" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G384" t="n">
         <v>3</v>
@@ -12351,7 +12351,7 @@
         <v>-0.1428571428571428</v>
       </c>
       <c r="F385" t="n">
-        <v>5.142857142857143</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G385" t="n">
         <v>1.142857142857143</v>
@@ -12382,7 +12382,7 @@
         <v>17</v>
       </c>
       <c r="F386" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G386" t="n">
         <v>1</v>
@@ -12413,7 +12413,7 @@
         <v>-1</v>
       </c>
       <c r="F387" t="n">
-        <v>3.666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G387" t="n">
         <v>1.333333333333333</v>
@@ -12444,7 +12444,7 @@
         <v>4.2</v>
       </c>
       <c r="F388" t="n">
-        <v>7.6</v>
+        <v>1.6</v>
       </c>
       <c r="G388" t="n">
         <v>1.2</v>
@@ -12475,7 +12475,7 @@
         <v>-8.5</v>
       </c>
       <c r="F389" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G389" t="n">
         <v>1</v>
@@ -12506,7 +12506,7 @@
         <v>4.666666666666667</v>
       </c>
       <c r="F390" t="n">
-        <v>5.333333333333333</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G390" t="n">
         <v>1.333333333333333</v>
@@ -12537,7 +12537,7 @@
         <v>-4</v>
       </c>
       <c r="F391" t="n">
-        <v>5</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G391" t="n">
         <v>1.571428571428571</v>
@@ -12568,7 +12568,7 @@
         <v>2.5</v>
       </c>
       <c r="F392" t="n">
-        <v>5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G392" t="n">
         <v>1.333333333333333</v>
@@ -12599,7 +12599,7 @@
         <v>-3.5</v>
       </c>
       <c r="F393" t="n">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="G393" t="n">
         <v>1</v>
@@ -12630,7 +12630,7 @@
         <v>0.2727272727272727</v>
       </c>
       <c r="F394" t="n">
-        <v>4.090909090909091</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="G394" t="n">
         <v>1.090909090909091</v>
@@ -12661,7 +12661,7 @@
         <v>1.25</v>
       </c>
       <c r="F395" t="n">
-        <v>5.25</v>
+        <v>1</v>
       </c>
       <c r="G395" t="n">
         <v>1</v>
@@ -12692,7 +12692,7 @@
         <v>0.125</v>
       </c>
       <c r="F396" t="n">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="G396" t="n">
         <v>1.125</v>
@@ -12723,7 +12723,7 @@
         <v>-5</v>
       </c>
       <c r="F397" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G397" t="n">
         <v>2</v>
@@ -12754,7 +12754,7 @@
         <v>-0.2857142857142857</v>
       </c>
       <c r="F398" t="n">
-        <v>4</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G398" t="n">
         <v>1.142857142857143</v>
@@ -12785,7 +12785,7 @@
         <v>-8</v>
       </c>
       <c r="F399" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G399" t="n">
         <v>1</v>
@@ -12816,7 +12816,7 @@
         <v>1.692307692307692</v>
       </c>
       <c r="F400" t="n">
-        <v>4.153846153846154</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="G400" t="n">
         <v>1</v>
@@ -12847,7 +12847,7 @@
         <v>2.8</v>
       </c>
       <c r="F401" t="n">
-        <v>4.2</v>
+        <v>0.8</v>
       </c>
       <c r="G401" t="n">
         <v>1.4</v>
@@ -12878,7 +12878,7 @@
         <v>-9</v>
       </c>
       <c r="F402" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G402" t="n">
         <v>2</v>
@@ -12909,7 +12909,7 @@
         <v>-11</v>
       </c>
       <c r="F403" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G403" t="n">
         <v>6</v>
@@ -12940,7 +12940,7 @@
         <v>3.1</v>
       </c>
       <c r="F404" t="n">
-        <v>7.7</v>
+        <v>1.6</v>
       </c>
       <c r="G404" t="n">
         <v>1.7</v>
@@ -12971,7 +12971,7 @@
         <v>4</v>
       </c>
       <c r="F405" t="n">
-        <v>7.666666666666667</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G405" t="n">
         <v>2</v>
@@ -13002,7 +13002,7 @@
         <v>4</v>
       </c>
       <c r="F406" t="n">
-        <v>4.071428571428571</v>
+        <v>0.5</v>
       </c>
       <c r="G406" t="n">
         <v>1</v>
@@ -13033,7 +13033,7 @@
         <v>-3</v>
       </c>
       <c r="F407" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G407" t="n">
         <v>3</v>
@@ -13064,7 +13064,7 @@
         <v>5</v>
       </c>
       <c r="F408" t="n">
-        <v>6</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G408" t="n">
         <v>1.333333333333333</v>
@@ -13095,7 +13095,7 @@
         <v>-1.333333333333333</v>
       </c>
       <c r="F409" t="n">
-        <v>4.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G409" t="n">
         <v>1.333333333333333</v>
@@ -13126,7 +13126,7 @@
         <v>4.714285714285714</v>
       </c>
       <c r="F410" t="n">
-        <v>4.142857142857143</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="G410" t="n">
         <v>1</v>
@@ -13157,7 +13157,7 @@
         <v>2.1</v>
       </c>
       <c r="F411" t="n">
-        <v>6.1</v>
+        <v>1.4</v>
       </c>
       <c r="G411" t="n">
         <v>1.5</v>
@@ -13188,7 +13188,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="F412" t="n">
-        <v>5.933333333333334</v>
+        <v>1.266666666666667</v>
       </c>
       <c r="G412" t="n">
         <v>1.4</v>
@@ -13219,7 +13219,7 @@
         <v>0</v>
       </c>
       <c r="F413" t="n">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="G413" t="n">
         <v>1</v>
@@ -13250,7 +13250,7 @@
         <v>5</v>
       </c>
       <c r="F414" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G414" t="n">
         <v>1</v>
@@ -13281,7 +13281,7 @@
         <v>1.375</v>
       </c>
       <c r="F415" t="n">
-        <v>4.125</v>
+        <v>1.125</v>
       </c>
       <c r="G415" t="n">
         <v>1</v>
@@ -13312,7 +13312,7 @@
         <v>3</v>
       </c>
       <c r="F416" t="n">
-        <v>5.285714285714286</v>
+        <v>1</v>
       </c>
       <c r="G416" t="n">
         <v>1</v>
@@ -13343,7 +13343,7 @@
         <v>1</v>
       </c>
       <c r="F417" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G417" t="n">
         <v>1.4</v>
@@ -13374,7 +13374,7 @@
         <v>1.5</v>
       </c>
       <c r="F418" t="n">
-        <v>3.833333333333333</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G418" t="n">
         <v>1.166666666666667</v>
@@ -13405,7 +13405,7 @@
         <v>2.666666666666667</v>
       </c>
       <c r="F419" t="n">
-        <v>5.833333333333333</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G419" t="n">
         <v>1.166666666666667</v>
@@ -13436,7 +13436,7 @@
         <v>1.368421052631579</v>
       </c>
       <c r="F420" t="n">
-        <v>5.526315789473684</v>
+        <v>1.236842105263158</v>
       </c>
       <c r="G420" t="n">
         <v>1.184210526315789</v>
@@ -13467,7 +13467,7 @@
         <v>5</v>
       </c>
       <c r="F421" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G421" t="n">
         <v>1</v>
@@ -13498,7 +13498,7 @@
         <v>4</v>
       </c>
       <c r="F422" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G422" t="n">
         <v>9</v>
@@ -13529,7 +13529,7 @@
         <v>2.054054054054054</v>
       </c>
       <c r="F423" t="n">
-        <v>4.432432432432432</v>
+        <v>0.9459459459459459</v>
       </c>
       <c r="G423" t="n">
         <v>1.027027027027027</v>
@@ -13560,7 +13560,7 @@
         <v>5.5</v>
       </c>
       <c r="F424" t="n">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="G424" t="n">
         <v>1</v>
@@ -13591,7 +13591,7 @@
         <v>-7</v>
       </c>
       <c r="F425" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G425" t="n">
         <v>1</v>
@@ -13622,7 +13622,7 @@
         <v>-2.25</v>
       </c>
       <c r="F426" t="n">
-        <v>7.75</v>
+        <v>1</v>
       </c>
       <c r="G426" t="n">
         <v>1.5</v>
@@ -13653,7 +13653,7 @@
         <v>1</v>
       </c>
       <c r="F427" t="n">
-        <v>3.8</v>
+        <v>0.6</v>
       </c>
       <c r="G427" t="n">
         <v>1</v>
@@ -13684,7 +13684,7 @@
         <v>3.166666666666667</v>
       </c>
       <c r="F428" t="n">
-        <v>4.833333333333333</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G428" t="n">
         <v>1.5</v>
@@ -13715,7 +13715,7 @@
         <v>-9</v>
       </c>
       <c r="F429" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G429" t="n">
         <v>1</v>
@@ -13746,7 +13746,7 @@
         <v>2.666666666666667</v>
       </c>
       <c r="F430" t="n">
-        <v>6.333333333333333</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G430" t="n">
         <v>1.333333333333333</v>
@@ -13777,7 +13777,7 @@
         <v>2</v>
       </c>
       <c r="F431" t="n">
-        <v>4.6</v>
+        <v>0.8</v>
       </c>
       <c r="G431" t="n">
         <v>1</v>
@@ -13808,7 +13808,7 @@
         <v>5.6</v>
       </c>
       <c r="F432" t="n">
-        <v>4.8</v>
+        <v>1.2</v>
       </c>
       <c r="G432" t="n">
         <v>1</v>
@@ -13839,7 +13839,7 @@
         <v>1.375</v>
       </c>
       <c r="F433" t="n">
-        <v>5.375</v>
+        <v>0.875</v>
       </c>
       <c r="G433" t="n">
         <v>1.375</v>
@@ -13870,7 +13870,7 @@
         <v>2.5</v>
       </c>
       <c r="F434" t="n">
-        <v>3.25</v>
+        <v>0.25</v>
       </c>
       <c r="G434" t="n">
         <v>1.25</v>
@@ -13901,7 +13901,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="F435" t="n">
-        <v>4.666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G435" t="n">
         <v>1.666666666666667</v>
@@ -13932,7 +13932,7 @@
         <v>3</v>
       </c>
       <c r="F436" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="G436" t="n">
         <v>9</v>
@@ -13963,7 +13963,7 @@
         <v>-0.8333333333333334</v>
       </c>
       <c r="F437" t="n">
-        <v>5.166666666666667</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G437" t="n">
         <v>1.166666666666667</v>
@@ -13994,7 +13994,7 @@
         <v>2.5</v>
       </c>
       <c r="F438" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G438" t="n">
         <v>6</v>
@@ -14025,7 +14025,7 @@
         <v>-1.5</v>
       </c>
       <c r="F439" t="n">
-        <v>6</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G439" t="n">
         <v>1.333333333333333</v>
@@ -14056,7 +14056,7 @@
         <v>-3</v>
       </c>
       <c r="F440" t="n">
-        <v>14.66666666666667</v>
+        <v>5</v>
       </c>
       <c r="G440" t="n">
         <v>2.333333333333333</v>
@@ -14087,7 +14087,7 @@
         <v>0.4444444444444444</v>
       </c>
       <c r="F441" t="n">
-        <v>4.222222222222222</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G441" t="n">
         <v>1.111111111111111</v>
@@ -14118,7 +14118,7 @@
         <v>-5</v>
       </c>
       <c r="F442" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G442" t="n">
         <v>2</v>
@@ -14149,7 +14149,7 @@
         <v>4.333333333333333</v>
       </c>
       <c r="F443" t="n">
-        <v>4.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G443" t="n">
         <v>1</v>
@@ -14180,7 +14180,7 @@
         <v>-0.3333333333333333</v>
       </c>
       <c r="F444" t="n">
-        <v>14</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="G444" t="n">
         <v>2.666666666666667</v>
@@ -14211,7 +14211,7 @@
         <v>-1.333333333333333</v>
       </c>
       <c r="F445" t="n">
-        <v>16</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G445" t="n">
         <v>4</v>
@@ -14242,7 +14242,7 @@
         <v>2.25</v>
       </c>
       <c r="F446" t="n">
-        <v>4.8125</v>
+        <v>0.75</v>
       </c>
       <c r="G446" t="n">
         <v>1.125</v>
@@ -14273,7 +14273,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="F447" t="n">
-        <v>5.833333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G447" t="n">
         <v>1.166666666666667</v>
@@ -14304,7 +14304,7 @@
         <v>4</v>
       </c>
       <c r="F448" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="G448" t="n">
         <v>9</v>
@@ -14335,7 +14335,7 @@
         <v>0.25</v>
       </c>
       <c r="F449" t="n">
-        <v>2.75</v>
+        <v>0.75</v>
       </c>
       <c r="G449" t="n">
         <v>1</v>
@@ -14366,7 +14366,7 @@
         <v>2</v>
       </c>
       <c r="F450" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G450" t="n">
         <v>1</v>
@@ -14397,7 +14397,7 @@
         <v>4</v>
       </c>
       <c r="F451" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="G451" t="n">
         <v>9</v>
@@ -14428,7 +14428,7 @@
         <v>0.625</v>
       </c>
       <c r="F452" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="G452" t="n">
         <v>1.125</v>
@@ -14459,7 +14459,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="F453" t="n">
-        <v>4.25</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="G453" t="n">
         <v>1.083333333333333</v>
@@ -14490,7 +14490,7 @@
         <v>1</v>
       </c>
       <c r="F454" t="n">
-        <v>6.142857142857143</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G454" t="n">
         <v>1.428571428571429</v>
@@ -14521,7 +14521,7 @@
         <v>0.7272727272727273</v>
       </c>
       <c r="F455" t="n">
-        <v>4.545454545454546</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="G455" t="n">
         <v>1.090909090909091</v>
@@ -14552,7 +14552,7 @@
         <v>-3</v>
       </c>
       <c r="F456" t="n">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="G456" t="n">
         <v>2</v>
@@ -14583,7 +14583,7 @@
         <v>9</v>
       </c>
       <c r="F457" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G457" t="n">
         <v>3</v>
@@ -14614,7 +14614,7 @@
         <v>-3.8</v>
       </c>
       <c r="F458" t="n">
-        <v>4.6</v>
+        <v>0.8</v>
       </c>
       <c r="G458" t="n">
         <v>1.2</v>
@@ -14645,7 +14645,7 @@
         <v>-12.5</v>
       </c>
       <c r="F459" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="G459" t="n">
         <v>1</v>
@@ -14676,7 +14676,7 @@
         <v>1.91044776119403</v>
       </c>
       <c r="F460" t="n">
-        <v>3.746268656716418</v>
+        <v>0.9253731343283582</v>
       </c>
       <c r="G460" t="n">
         <v>1.164179104477612</v>
@@ -14707,7 +14707,7 @@
         <v>-0.6666666666666666</v>
       </c>
       <c r="F461" t="n">
-        <v>12.55555555555556</v>
+        <v>2.888888888888889</v>
       </c>
       <c r="G461" t="n">
         <v>3</v>
@@ -14738,7 +14738,7 @@
         <v>-3.5</v>
       </c>
       <c r="F462" t="n">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="G462" t="n">
         <v>1</v>
@@ -14769,7 +14769,7 @@
         <v>1.823529411764706</v>
       </c>
       <c r="F463" t="n">
-        <v>6.823529411764706</v>
+        <v>1.588235294117647</v>
       </c>
       <c r="G463" t="n">
         <v>1.647058823529412</v>
@@ -14800,7 +14800,7 @@
         <v>5</v>
       </c>
       <c r="F464" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G464" t="n">
         <v>9</v>
@@ -14831,7 +14831,7 @@
         <v>2</v>
       </c>
       <c r="F465" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G465" t="n">
         <v>3</v>
@@ -14862,7 +14862,7 @@
         <v>0</v>
       </c>
       <c r="F466" t="n">
-        <v>4.571428571428571</v>
+        <v>1</v>
       </c>
       <c r="G466" t="n">
         <v>1</v>
@@ -14893,7 +14893,7 @@
         <v>3</v>
       </c>
       <c r="F467" t="n">
-        <v>31</v>
+        <v>6.5</v>
       </c>
       <c r="G467" t="n">
         <v>9</v>
@@ -14924,7 +14924,7 @@
         <v>-2</v>
       </c>
       <c r="F468" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G468" t="n">
         <v>1</v>
@@ -14955,7 +14955,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F469" t="n">
-        <v>3.666666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G469" t="n">
         <v>1</v>
@@ -14986,7 +14986,7 @@
         <v>-10</v>
       </c>
       <c r="F470" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G470" t="n">
         <v>1</v>
@@ -15017,7 +15017,7 @@
         <v>-6</v>
       </c>
       <c r="F471" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G471" t="n">
         <v>4</v>
@@ -15048,7 +15048,7 @@
         <v>0.7272727272727273</v>
       </c>
       <c r="F472" t="n">
-        <v>5.363636363636363</v>
+        <v>1.272727272727273</v>
       </c>
       <c r="G472" t="n">
         <v>1</v>
@@ -15079,7 +15079,7 @@
         <v>0.4</v>
       </c>
       <c r="F473" t="n">
-        <v>3.7</v>
+        <v>0.6</v>
       </c>
       <c r="G473" t="n">
         <v>1.5</v>
@@ -15110,7 +15110,7 @@
         <v>1.5</v>
       </c>
       <c r="F474" t="n">
-        <v>5.625</v>
+        <v>1.5</v>
       </c>
       <c r="G474" t="n">
         <v>1.375</v>
@@ -15141,7 +15141,7 @@
         <v>0</v>
       </c>
       <c r="F475" t="n">
-        <v>14</v>
+        <v>4.5</v>
       </c>
       <c r="G475" t="n">
         <v>3.5</v>
@@ -15172,7 +15172,7 @@
         <v>0.5</v>
       </c>
       <c r="F476" t="n">
-        <v>4.8</v>
+        <v>1</v>
       </c>
       <c r="G476" t="n">
         <v>1</v>
@@ -15203,7 +15203,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="F477" t="n">
-        <v>5.083333333333333</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G477" t="n">
         <v>1.5</v>
@@ -15234,7 +15234,7 @@
         <v>2.076923076923077</v>
       </c>
       <c r="F478" t="n">
-        <v>7.384615384615385</v>
+        <v>1.615384615384615</v>
       </c>
       <c r="G478" t="n">
         <v>1.615384615384615</v>
@@ -15265,7 +15265,7 @@
         <v>5</v>
       </c>
       <c r="F479" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G479" t="n">
         <v>1</v>
@@ -15296,7 +15296,7 @@
         <v>-4.25</v>
       </c>
       <c r="F480" t="n">
-        <v>8.75</v>
+        <v>2</v>
       </c>
       <c r="G480" t="n">
         <v>2.5</v>
@@ -15327,7 +15327,7 @@
         <v>1</v>
       </c>
       <c r="F481" t="n">
-        <v>6.7</v>
+        <v>1.7</v>
       </c>
       <c r="G481" t="n">
         <v>1.3</v>
@@ -15358,7 +15358,7 @@
         <v>0</v>
       </c>
       <c r="F482" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="G482" t="n">
         <v>1</v>
@@ -15389,7 +15389,7 @@
         <v>6</v>
       </c>
       <c r="F483" t="n">
-        <v>6.5</v>
+        <v>1.25</v>
       </c>
       <c r="G483" t="n">
         <v>1.25</v>
@@ -15420,7 +15420,7 @@
         <v>-6</v>
       </c>
       <c r="F484" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G484" t="n">
         <v>2</v>
@@ -15451,7 +15451,7 @@
         <v>1.1</v>
       </c>
       <c r="F485" t="n">
-        <v>7.3</v>
+        <v>1.9</v>
       </c>
       <c r="G485" t="n">
         <v>1.7</v>
@@ -15482,7 +15482,7 @@
         <v>-1</v>
       </c>
       <c r="F486" t="n">
-        <v>11.85714285714286</v>
+        <v>2</v>
       </c>
       <c r="G486" t="n">
         <v>3.428571428571428</v>
@@ -15513,7 +15513,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="F487" t="n">
-        <v>5.666666666666667</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G487" t="n">
         <v>1</v>
@@ -15544,7 +15544,7 @@
         <v>5</v>
       </c>
       <c r="F488" t="n">
-        <v>36.5</v>
+        <v>6.5</v>
       </c>
       <c r="G488" t="n">
         <v>9</v>
@@ -15575,7 +15575,7 @@
         <v>-10.5</v>
       </c>
       <c r="F489" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G489" t="n">
         <v>1</v>
@@ -15606,7 +15606,7 @@
         <v>2</v>
       </c>
       <c r="F490" t="n">
-        <v>4.75</v>
+        <v>0.25</v>
       </c>
       <c r="G490" t="n">
         <v>1.25</v>
@@ -15637,7 +15637,7 @@
         <v>5</v>
       </c>
       <c r="F491" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G491" t="n">
         <v>2</v>
@@ -15668,7 +15668,7 @@
         <v>-5</v>
       </c>
       <c r="F492" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G492" t="n">
         <v>1</v>
@@ -15699,7 +15699,7 @@
         <v>1.5</v>
       </c>
       <c r="F493" t="n">
-        <v>3.75</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="G493" t="n">
         <v>1.083333333333333</v>
@@ -15730,7 +15730,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="F494" t="n">
-        <v>5.5</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="G494" t="n">
         <v>1.333333333333333</v>
@@ -15761,7 +15761,7 @@
         <v>-1.571428571428571</v>
       </c>
       <c r="F495" t="n">
-        <v>5.571428571428571</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="G495" t="n">
         <v>1.285714285714286</v>
@@ -15792,7 +15792,7 @@
         <v>5.727272727272728</v>
       </c>
       <c r="F496" t="n">
-        <v>7.636363636363637</v>
+        <v>1.545454545454545</v>
       </c>
       <c r="G496" t="n">
         <v>1.363636363636364</v>
@@ -15823,7 +15823,7 @@
         <v>0.8421052631578947</v>
       </c>
       <c r="F497" t="n">
-        <v>5.105263157894737</v>
+        <v>1.052631578947368</v>
       </c>
       <c r="G497" t="n">
         <v>1.157894736842105</v>
@@ -15854,7 +15854,7 @@
         <v>1</v>
       </c>
       <c r="F498" t="n">
-        <v>4.583333333333333</v>
+        <v>1.083333333333333</v>
       </c>
       <c r="G498" t="n">
         <v>1.083333333333333</v>
@@ -15885,7 +15885,7 @@
         <v>1.523809523809524</v>
       </c>
       <c r="F499" t="n">
-        <v>5.714285714285714</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="G499" t="n">
         <v>1.142857142857143</v>
@@ -15916,7 +15916,7 @@
         <v>-5</v>
       </c>
       <c r="F500" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G500" t="n">
         <v>1.5</v>
@@ -15947,7 +15947,7 @@
         <v>-8</v>
       </c>
       <c r="F501" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G501" t="n">
         <v>1</v>
@@ -15978,7 +15978,7 @@
         <v>4</v>
       </c>
       <c r="F502" t="n">
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="G502" t="n">
         <v>2</v>
@@ -16009,7 +16009,7 @@
         <v>0.9523809523809523</v>
       </c>
       <c r="F503" t="n">
-        <v>6.619047619047619</v>
+        <v>1.904761904761905</v>
       </c>
       <c r="G503" t="n">
         <v>1.666666666666667</v>
@@ -16040,7 +16040,7 @@
         <v>0</v>
       </c>
       <c r="F504" t="n">
-        <v>4.857142857142857</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="G504" t="n">
         <v>1.142857142857143</v>
@@ -16071,7 +16071,7 @@
         <v>1</v>
       </c>
       <c r="F505" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="G505" t="n">
         <v>9</v>
@@ -16102,7 +16102,7 @@
         <v>1</v>
       </c>
       <c r="F506" t="n">
-        <v>4</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G506" t="n">
         <v>1.142857142857143</v>
@@ -16133,7 +16133,7 @@
         <v>1.909090909090909</v>
       </c>
       <c r="F507" t="n">
-        <v>4.636363636363637</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="G507" t="n">
         <v>1.272727272727273</v>
@@ -16164,7 +16164,7 @@
         <v>1</v>
       </c>
       <c r="F508" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G508" t="n">
         <v>4</v>
@@ -16195,7 +16195,7 @@
         <v>3.818181818181818</v>
       </c>
       <c r="F509" t="n">
-        <v>6.272727272727272</v>
+        <v>1.545454545454545</v>
       </c>
       <c r="G509" t="n">
         <v>1.545454545454545</v>
@@ -16226,7 +16226,7 @@
         <v>4</v>
       </c>
       <c r="F510" t="n">
-        <v>11.5</v>
+        <v>2.5</v>
       </c>
       <c r="G510" t="n">
         <v>4</v>
@@ -16257,7 +16257,7 @@
         <v>-1.25</v>
       </c>
       <c r="F511" t="n">
-        <v>7.75</v>
+        <v>1</v>
       </c>
       <c r="G511" t="n">
         <v>1.75</v>
@@ -16288,7 +16288,7 @@
         <v>-1</v>
       </c>
       <c r="F512" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G512" t="n">
         <v>1</v>
@@ -16319,7 +16319,7 @@
         <v>4</v>
       </c>
       <c r="F513" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G513" t="n">
         <v>5</v>
@@ -16350,7 +16350,7 @@
         <v>1.636363636363636</v>
       </c>
       <c r="F514" t="n">
-        <v>6.090909090909091</v>
+        <v>1.681818181818182</v>
       </c>
       <c r="G514" t="n">
         <v>1</v>
@@ -16381,7 +16381,7 @@
         <v>-9.333333333333334</v>
       </c>
       <c r="F515" t="n">
-        <v>3.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G515" t="n">
         <v>1.333333333333333</v>
@@ -16412,7 +16412,7 @@
         <v>2</v>
       </c>
       <c r="F516" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G516" t="n">
         <v>1</v>
@@ -16443,7 +16443,7 @@
         <v>-10</v>
       </c>
       <c r="F517" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G517" t="n">
         <v>1</v>
@@ -16474,7 +16474,7 @@
         <v>2.090909090909091</v>
       </c>
       <c r="F518" t="n">
-        <v>4.090909090909091</v>
+        <v>1.090909090909091</v>
       </c>
       <c r="G518" t="n">
         <v>1</v>
@@ -16505,7 +16505,7 @@
         <v>1.6</v>
       </c>
       <c r="F519" t="n">
-        <v>5.3</v>
+        <v>1.1</v>
       </c>
       <c r="G519" t="n">
         <v>1.2</v>
@@ -16536,7 +16536,7 @@
         <v>1</v>
       </c>
       <c r="F520" t="n">
-        <v>7.4</v>
+        <v>1.6</v>
       </c>
       <c r="G520" t="n">
         <v>1.8</v>
@@ -16567,7 +16567,7 @@
         <v>-0.5</v>
       </c>
       <c r="F521" t="n">
-        <v>10.3</v>
+        <v>2.2</v>
       </c>
       <c r="G521" t="n">
         <v>2.4</v>
@@ -16598,7 +16598,7 @@
         <v>4.5</v>
       </c>
       <c r="F522" t="n">
-        <v>9.5</v>
+        <v>2.5</v>
       </c>
       <c r="G522" t="n">
         <v>2</v>
@@ -16629,7 +16629,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="F523" t="n">
-        <v>5.166666666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G523" t="n">
         <v>1</v>
@@ -16660,7 +16660,7 @@
         <v>-2</v>
       </c>
       <c r="F524" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G524" t="n">
         <v>2</v>
@@ -16691,7 +16691,7 @@
         <v>-2</v>
       </c>
       <c r="F525" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G525" t="n">
         <v>2</v>
@@ -16722,7 +16722,7 @@
         <v>3.166666666666667</v>
       </c>
       <c r="F526" t="n">
-        <v>5.666666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G526" t="n">
         <v>1.833333333333333</v>
@@ -16753,7 +16753,7 @@
         <v>-11</v>
       </c>
       <c r="F527" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G527" t="n">
         <v>1</v>
@@ -16784,7 +16784,7 @@
         <v>1.481481481481481</v>
       </c>
       <c r="F528" t="n">
-        <v>5.444444444444445</v>
+        <v>1.37037037037037</v>
       </c>
       <c r="G528" t="n">
         <v>1.111111111111111</v>
@@ -16815,7 +16815,7 @@
         <v>2.75</v>
       </c>
       <c r="F529" t="n">
-        <v>5.5</v>
+        <v>1.25</v>
       </c>
       <c r="G529" t="n">
         <v>1</v>
@@ -16846,7 +16846,7 @@
         <v>-1.571428571428571</v>
       </c>
       <c r="F530" t="n">
-        <v>8.714285714285714</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="G530" t="n">
         <v>1.571428571428571</v>
@@ -16877,7 +16877,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="F531" t="n">
-        <v>5.666666666666667</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="G531" t="n">
         <v>1.333333333333333</v>
@@ -16908,7 +16908,7 @@
         <v>-2.4</v>
       </c>
       <c r="F532" t="n">
-        <v>4.6</v>
+        <v>0.8</v>
       </c>
       <c r="G532" t="n">
         <v>1.2</v>
@@ -16939,7 +16939,7 @@
         <v>-1</v>
       </c>
       <c r="F533" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G533" t="n">
         <v>1</v>
@@ -16970,7 +16970,7 @@
         <v>-0.6666666666666666</v>
       </c>
       <c r="F534" t="n">
-        <v>5.166666666666667</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="G534" t="n">
         <v>1.666666666666667</v>
@@ -16989,25 +16989,25 @@
         </is>
       </c>
       <c r="B535" t="n">
-        <v>2.112069813341116</v>
+        <v>2.112243226672423</v>
       </c>
       <c r="C535" t="n">
-        <v>23.91903798177617</v>
+        <v>23.9192487359343</v>
       </c>
       <c r="D535" t="n">
-        <v>0.3684035500885393</v>
+        <v>0.3684276001125894</v>
       </c>
       <c r="E535" t="n">
-        <v>0.1599043236361397</v>
+        <v>0.159799895900133</v>
       </c>
       <c r="F535" t="n">
-        <v>6.906454591502478</v>
+        <v>1.448562904744733</v>
       </c>
       <c r="G535" t="n">
-        <v>1.79647149858344</v>
+        <v>1.796504409142666</v>
       </c>
       <c r="H535" t="n">
-        <v>8.203528501416558</v>
+        <v>8.203495590857333</v>
       </c>
       <c r="I535" t="n">
         <v>9</v>

</xml_diff>